<commit_message>
Update GIOVINAZZO CENSIMENTO VERDE_2022.xlsx
</commit_message>
<xml_diff>
--- a/GIOVINAZZO CENSIMENTO VERDE_2022.xlsx
+++ b/GIOVINAZZO CENSIMENTO VERDE_2022.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\daniele.tarantino\Documents\GitHub\CensimentoVerde\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAFBE150-4A29-4C3E-A834-904BE99B6D42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA06F521-0C12-4BA7-8094-7766C2D04AC9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -597,9 +597,6 @@
     <t>Potatura e Manutenzione</t>
   </si>
   <si>
-    <t>x</t>
-  </si>
-  <si>
     <t>Sostituiti n.5 Tamerici secchi con n.5 Tamerici</t>
   </si>
   <si>
@@ -617,6 +614,9 @@
   <si>
     <t>Potatura di alleggerimento di n. 5 Carrubi
 con successivo sostegno in legno</t>
+  </si>
+  <si>
+    <t>(n.7)</t>
   </si>
 </sst>
 </file>
@@ -1127,51 +1127,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1220,6 +1175,51 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1563,9 +1563,9 @@
   <dimension ref="A1:I258"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A4" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <pane ySplit="6" topLeftCell="A144" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="6" topLeftCell="A33" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="A4" sqref="A4"/>
-      <selection pane="bottomLeft" activeCell="F240" sqref="F240"/>
+      <selection pane="bottomLeft" activeCell="D47" sqref="D47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1582,74 +1582,74 @@
       <c r="A1" s="3"/>
       <c r="B1" s="48"/>
       <c r="C1" s="4"/>
-      <c r="D1" s="88"/>
-      <c r="E1" s="88"/>
+      <c r="D1" s="71"/>
+      <c r="E1" s="71"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A2" s="71" t="s">
+      <c r="A2" s="101" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="71"/>
-      <c r="C2" s="71"/>
-      <c r="D2" s="89"/>
-      <c r="E2" s="89"/>
+      <c r="B2" s="101"/>
+      <c r="C2" s="101"/>
+      <c r="D2" s="72"/>
+      <c r="E2" s="72"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A3" s="72" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" s="72"/>
-      <c r="C3" s="72"/>
-      <c r="D3" s="90"/>
-      <c r="E3" s="90"/>
+      <c r="A3" s="102" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="102"/>
+      <c r="C3" s="102"/>
+      <c r="D3" s="73"/>
+      <c r="E3" s="73"/>
     </row>
     <row r="4" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="87" t="s">
+      <c r="A4" s="88" t="s">
         <v>161</v>
       </c>
-      <c r="B4" s="87"/>
-      <c r="C4" s="87"/>
-      <c r="D4" s="87"/>
-      <c r="E4" s="87"/>
-      <c r="F4" s="87"/>
+      <c r="B4" s="88"/>
+      <c r="C4" s="88"/>
+      <c r="D4" s="88"/>
+      <c r="E4" s="88"/>
+      <c r="F4" s="88"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A5" s="87"/>
-      <c r="B5" s="87"/>
-      <c r="C5" s="87"/>
-      <c r="D5" s="87"/>
-      <c r="E5" s="87"/>
-      <c r="F5" s="87"/>
+      <c r="A5" s="88"/>
+      <c r="B5" s="88"/>
+      <c r="C5" s="88"/>
+      <c r="D5" s="88"/>
+      <c r="E5" s="88"/>
+      <c r="F5" s="88"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A6" s="87"/>
-      <c r="B6" s="87"/>
-      <c r="C6" s="87"/>
-      <c r="D6" s="87"/>
-      <c r="E6" s="87"/>
-      <c r="F6" s="87"/>
+      <c r="A6" s="88"/>
+      <c r="B6" s="88"/>
+      <c r="C6" s="88"/>
+      <c r="D6" s="88"/>
+      <c r="E6" s="88"/>
+      <c r="F6" s="88"/>
       <c r="G6" s="21"/>
       <c r="H6" s="21"/>
       <c r="I6" s="21"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A7" s="87"/>
-      <c r="B7" s="87"/>
-      <c r="C7" s="87"/>
-      <c r="D7" s="87"/>
-      <c r="E7" s="87"/>
-      <c r="F7" s="87"/>
+      <c r="A7" s="88"/>
+      <c r="B7" s="88"/>
+      <c r="C7" s="88"/>
+      <c r="D7" s="88"/>
+      <c r="E7" s="88"/>
+      <c r="F7" s="88"/>
       <c r="G7" s="21"/>
       <c r="H7" s="21"/>
       <c r="I7" s="21"/>
     </row>
     <row r="8" spans="1:9" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="87"/>
-      <c r="B8" s="87"/>
-      <c r="C8" s="87"/>
-      <c r="D8" s="87"/>
-      <c r="E8" s="87"/>
-      <c r="F8" s="87"/>
+      <c r="A8" s="88"/>
+      <c r="B8" s="88"/>
+      <c r="C8" s="88"/>
+      <c r="D8" s="88"/>
+      <c r="E8" s="88"/>
+      <c r="F8" s="88"/>
       <c r="G8" s="21"/>
       <c r="H8" s="21"/>
       <c r="I8" s="21"/>
@@ -1684,8 +1684,8 @@
       <c r="C10" s="7">
         <v>108</v>
       </c>
-      <c r="D10" s="91"/>
-      <c r="E10" s="91"/>
+      <c r="D10" s="74"/>
+      <c r="E10" s="74"/>
     </row>
     <row r="11" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="1"/>
@@ -1695,8 +1695,8 @@
       <c r="C11" s="7">
         <v>1</v>
       </c>
-      <c r="D11" s="91"/>
-      <c r="E11" s="91"/>
+      <c r="D11" s="74"/>
+      <c r="E11" s="74"/>
     </row>
     <row r="12" spans="1:9" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A12" s="1"/>
@@ -1706,8 +1706,8 @@
       <c r="C12" s="7">
         <v>9</v>
       </c>
-      <c r="D12" s="91"/>
-      <c r="E12" s="91"/>
+      <c r="D12" s="74"/>
+      <c r="E12" s="74"/>
     </row>
     <row r="13" spans="1:9" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A13" s="1"/>
@@ -1717,8 +1717,8 @@
       <c r="C13" s="7">
         <v>6</v>
       </c>
-      <c r="D13" s="91"/>
-      <c r="E13" s="91"/>
+      <c r="D13" s="74"/>
+      <c r="E13" s="74"/>
     </row>
     <row r="14" spans="1:9" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A14" s="1"/>
@@ -1726,11 +1726,11 @@
         <v>126</v>
       </c>
       <c r="C14" s="7"/>
-      <c r="D14" s="91"/>
-      <c r="E14" s="91"/>
+      <c r="D14" s="74"/>
+      <c r="E14" s="74"/>
     </row>
     <row r="15" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="77" t="s">
+      <c r="A15" s="89" t="s">
         <v>6</v>
       </c>
       <c r="B15" s="9" t="s">
@@ -1739,19 +1739,19 @@
       <c r="C15" s="6">
         <v>21</v>
       </c>
-      <c r="D15" s="92"/>
-      <c r="E15" s="92"/>
+      <c r="D15" s="75"/>
+      <c r="E15" s="75"/>
     </row>
     <row r="16" spans="1:9" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A16" s="75"/>
+      <c r="A16" s="90"/>
       <c r="B16" s="27" t="s">
         <v>103</v>
       </c>
       <c r="C16" s="6">
         <v>1</v>
       </c>
-      <c r="D16" s="92"/>
-      <c r="E16" s="92"/>
+      <c r="D16" s="75"/>
+      <c r="E16" s="75"/>
     </row>
     <row r="17" spans="1:5" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
@@ -1763,8 +1763,8 @@
       <c r="C17" s="6">
         <v>33</v>
       </c>
-      <c r="D17" s="92"/>
-      <c r="E17" s="92"/>
+      <c r="D17" s="75"/>
+      <c r="E17" s="75"/>
     </row>
     <row r="18" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A18" s="1"/>
@@ -1774,8 +1774,8 @@
       <c r="C18" s="6">
         <v>31</v>
       </c>
-      <c r="D18" s="92"/>
-      <c r="E18" s="92"/>
+      <c r="D18" s="75"/>
+      <c r="E18" s="75"/>
     </row>
     <row r="19" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A19" s="1"/>
@@ -1785,8 +1785,8 @@
       <c r="C19" s="6">
         <v>10</v>
       </c>
-      <c r="D19" s="92"/>
-      <c r="E19" s="92"/>
+      <c r="D19" s="75"/>
+      <c r="E19" s="75"/>
     </row>
     <row r="20" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A20" s="3"/>
@@ -1794,8 +1794,8 @@
         <v>94</v>
       </c>
       <c r="C20" s="60"/>
-      <c r="D20" s="93"/>
-      <c r="E20" s="93"/>
+      <c r="D20" s="76"/>
+      <c r="E20" s="76"/>
     </row>
     <row r="21" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
@@ -1807,11 +1807,11 @@
       <c r="C21" s="6">
         <v>10</v>
       </c>
-      <c r="D21" s="92"/>
-      <c r="E21" s="92"/>
+      <c r="D21" s="75"/>
+      <c r="E21" s="75"/>
     </row>
     <row r="22" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="77" t="s">
+      <c r="A22" s="89" t="s">
         <v>152</v>
       </c>
       <c r="B22" s="32" t="s">
@@ -1820,19 +1820,19 @@
       <c r="C22" s="6">
         <v>8</v>
       </c>
-      <c r="D22" s="92"/>
-      <c r="E22" s="92"/>
+      <c r="D22" s="75"/>
+      <c r="E22" s="75"/>
     </row>
     <row r="23" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A23" s="75"/>
+      <c r="A23" s="90"/>
       <c r="B23" s="12" t="s">
         <v>110</v>
       </c>
       <c r="C23" s="6">
         <v>2</v>
       </c>
-      <c r="D23" s="92"/>
-      <c r="E23" s="92"/>
+      <c r="D23" s="75"/>
+      <c r="E23" s="75"/>
     </row>
     <row r="24" spans="1:5" ht="57" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
@@ -1844,9 +1844,9 @@
       <c r="C24" s="6">
         <v>36</v>
       </c>
-      <c r="D24" s="92"/>
-      <c r="E24" s="92" t="s">
-        <v>170</v>
+      <c r="D24" s="75"/>
+      <c r="E24" s="75" t="s">
+        <v>169</v>
       </c>
     </row>
     <row r="25" spans="1:5" ht="57.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1859,13 +1859,13 @@
       <c r="C25" s="6">
         <v>123</v>
       </c>
-      <c r="D25" s="92"/>
-      <c r="E25" s="92" t="s">
-        <v>170</v>
+      <c r="D25" s="75"/>
+      <c r="E25" s="75" t="s">
+        <v>169</v>
       </c>
     </row>
     <row r="26" spans="1:5" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="77" t="s">
+      <c r="A26" s="89" t="s">
         <v>10</v>
       </c>
       <c r="B26" s="61" t="s">
@@ -1874,19 +1874,19 @@
       <c r="C26" s="7">
         <v>18</v>
       </c>
-      <c r="D26" s="91"/>
-      <c r="E26" s="91"/>
+      <c r="D26" s="74"/>
+      <c r="E26" s="74"/>
     </row>
     <row r="27" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="75"/>
+      <c r="A27" s="90"/>
       <c r="B27" s="25" t="s">
         <v>109</v>
       </c>
       <c r="C27" s="6">
         <v>3</v>
       </c>
-      <c r="D27" s="92"/>
-      <c r="E27" s="92"/>
+      <c r="D27" s="75"/>
+      <c r="E27" s="75"/>
     </row>
     <row r="28" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
@@ -1898,11 +1898,11 @@
       <c r="C28" s="6">
         <v>17</v>
       </c>
-      <c r="D28" s="92"/>
-      <c r="E28" s="92"/>
+      <c r="D28" s="75"/>
+      <c r="E28" s="75"/>
     </row>
     <row r="29" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A29" s="77" t="s">
+      <c r="A29" s="89" t="s">
         <v>13</v>
       </c>
       <c r="B29" s="33" t="s">
@@ -1911,33 +1911,33 @@
       <c r="C29" s="6">
         <v>1</v>
       </c>
-      <c r="D29" s="92"/>
-      <c r="E29" s="92"/>
+      <c r="D29" s="75"/>
+      <c r="E29" s="75"/>
     </row>
     <row r="30" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A30" s="75"/>
+      <c r="A30" s="90"/>
       <c r="B30" s="25" t="s">
         <v>109</v>
       </c>
       <c r="C30" s="6">
         <v>7</v>
       </c>
-      <c r="D30" s="92"/>
-      <c r="E30" s="92"/>
+      <c r="D30" s="75"/>
+      <c r="E30" s="75"/>
     </row>
     <row r="31" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A31" s="75"/>
+      <c r="A31" s="90"/>
       <c r="B31" s="32" t="s">
         <v>108</v>
       </c>
       <c r="C31" s="6">
         <v>7</v>
       </c>
-      <c r="D31" s="92"/>
-      <c r="E31" s="92"/>
+      <c r="D31" s="75"/>
+      <c r="E31" s="75"/>
     </row>
     <row r="32" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A32" s="77" t="s">
+      <c r="A32" s="89" t="s">
         <v>14</v>
       </c>
       <c r="B32" s="33" t="s">
@@ -1946,22 +1946,22 @@
       <c r="C32" s="6">
         <v>1</v>
       </c>
-      <c r="D32" s="92"/>
-      <c r="E32" s="92"/>
+      <c r="D32" s="75"/>
+      <c r="E32" s="75"/>
     </row>
     <row r="33" spans="1:6" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A33" s="75"/>
+      <c r="A33" s="90"/>
       <c r="B33" s="45" t="s">
         <v>140</v>
       </c>
       <c r="C33" s="6">
         <v>18</v>
       </c>
-      <c r="D33" s="92"/>
-      <c r="E33" s="92"/>
+      <c r="D33" s="75"/>
+      <c r="E33" s="75"/>
     </row>
     <row r="34" spans="1:6" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A34" s="83" t="s">
+      <c r="A34" s="93" t="s">
         <v>15</v>
       </c>
       <c r="B34" s="34" t="s">
@@ -1970,35 +1970,35 @@
       <c r="C34" s="6">
         <v>48</v>
       </c>
-      <c r="D34" s="92"/>
-      <c r="E34" s="92"/>
+      <c r="D34" s="75"/>
+      <c r="E34" s="75"/>
     </row>
     <row r="35" spans="1:6" ht="69.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="84"/>
+      <c r="A35" s="94"/>
       <c r="B35" s="26" t="s">
         <v>16</v>
       </c>
       <c r="C35" s="6">
         <v>44</v>
       </c>
-      <c r="D35" s="92"/>
-      <c r="E35" s="92" t="s">
+      <c r="D35" s="75"/>
+      <c r="E35" s="75" t="s">
+        <v>170</v>
+      </c>
+      <c r="F35" s="75" t="s">
         <v>171</v>
       </c>
-      <c r="F35" s="92" t="s">
-        <v>172</v>
-      </c>
     </row>
     <row r="36" spans="1:6" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A36" s="84"/>
+      <c r="A36" s="94"/>
       <c r="B36" s="23" t="s">
         <v>92</v>
       </c>
       <c r="C36" s="6">
         <v>1</v>
       </c>
-      <c r="D36" s="92"/>
-      <c r="E36" s="92"/>
+      <c r="D36" s="75"/>
+      <c r="E36" s="75"/>
       <c r="F36" s="70"/>
     </row>
     <row r="37" spans="1:6" ht="15.75" x14ac:dyDescent="0.2">
@@ -2011,12 +2011,12 @@
       <c r="C37" s="6">
         <v>9</v>
       </c>
-      <c r="D37" s="92"/>
-      <c r="E37" s="92"/>
+      <c r="D37" s="75"/>
+      <c r="E37" s="75"/>
       <c r="F37" s="70"/>
     </row>
     <row r="38" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="77" t="s">
+      <c r="A38" s="89" t="s">
         <v>18</v>
       </c>
       <c r="B38" s="12" t="s">
@@ -2025,26 +2025,26 @@
       <c r="C38" s="6">
         <v>2</v>
       </c>
-      <c r="D38" s="92"/>
-      <c r="E38" s="92"/>
+      <c r="D38" s="75"/>
+      <c r="E38" s="75"/>
     </row>
     <row r="39" spans="1:6" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A39" s="75"/>
+      <c r="A39" s="90"/>
       <c r="B39" s="27" t="s">
         <v>103</v>
       </c>
       <c r="C39" s="6">
         <v>1</v>
       </c>
-      <c r="D39" s="92"/>
-      <c r="E39" s="92"/>
+      <c r="D39" s="75"/>
+      <c r="E39" s="75"/>
     </row>
     <row r="40" spans="1:6" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A40" s="75"/>
+      <c r="A40" s="90"/>
       <c r="B40" s="23"/>
       <c r="C40" s="60"/>
-      <c r="D40" s="93"/>
-      <c r="E40" s="93"/>
+      <c r="D40" s="76"/>
+      <c r="E40" s="76"/>
     </row>
     <row r="41" spans="1:6" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
@@ -2056,8 +2056,8 @@
       <c r="C41" s="6">
         <v>14</v>
       </c>
-      <c r="D41" s="92"/>
-      <c r="E41" s="92"/>
+      <c r="D41" s="75"/>
+      <c r="E41" s="75"/>
     </row>
     <row r="42" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
@@ -2069,11 +2069,11 @@
       <c r="C42" s="6">
         <v>15</v>
       </c>
-      <c r="D42" s="92"/>
-      <c r="E42" s="92"/>
+      <c r="D42" s="75"/>
+      <c r="E42" s="75"/>
     </row>
     <row r="43" spans="1:6" ht="29.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="77" t="s">
+      <c r="A43" s="89" t="s">
         <v>22</v>
       </c>
       <c r="B43" s="42" t="s">
@@ -2082,19 +2082,19 @@
       <c r="C43" s="6">
         <v>7</v>
       </c>
-      <c r="D43" s="92"/>
-      <c r="E43" s="92"/>
+      <c r="D43" s="75"/>
+      <c r="E43" s="75"/>
     </row>
     <row r="44" spans="1:6" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A44" s="75"/>
+      <c r="A44" s="90"/>
       <c r="B44" s="30" t="s">
         <v>107</v>
       </c>
       <c r="C44" s="6">
         <v>32</v>
       </c>
-      <c r="D44" s="92"/>
-      <c r="E44" s="92"/>
+      <c r="D44" s="75"/>
+      <c r="E44" s="75"/>
     </row>
     <row r="45" spans="1:6" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
@@ -2106,11 +2106,11 @@
       <c r="C45" s="6">
         <v>10</v>
       </c>
-      <c r="D45" s="92"/>
-      <c r="E45" s="92"/>
+      <c r="D45" s="75"/>
+      <c r="E45" s="75"/>
     </row>
     <row r="46" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A46" s="77" t="s">
+      <c r="A46" s="89" t="s">
         <v>24</v>
       </c>
       <c r="B46" s="32" t="s">
@@ -2119,35 +2119,35 @@
       <c r="C46" s="6">
         <v>2</v>
       </c>
-      <c r="D46" s="92"/>
-      <c r="E46" s="92"/>
+      <c r="D46" s="75"/>
+      <c r="E46" s="75"/>
     </row>
     <row r="47" spans="1:6" s="70" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A47" s="77"/>
+      <c r="A47" s="89"/>
       <c r="B47" s="30" t="s">
         <v>107</v>
       </c>
       <c r="C47" s="65">
-        <v>4</v>
-      </c>
-      <c r="D47" s="92" t="s">
-        <v>169</v>
-      </c>
-      <c r="E47" s="92"/>
+        <v>7</v>
+      </c>
+      <c r="D47" s="75" t="s">
+        <v>174</v>
+      </c>
+      <c r="E47" s="75"/>
     </row>
     <row r="48" spans="1:6" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A48" s="75"/>
+      <c r="A48" s="90"/>
       <c r="B48" s="28" t="s">
         <v>111</v>
       </c>
       <c r="C48" s="6">
         <v>10</v>
       </c>
-      <c r="D48" s="92"/>
-      <c r="E48" s="92"/>
+      <c r="D48" s="75"/>
+      <c r="E48" s="75"/>
     </row>
     <row r="49" spans="1:5" ht="33" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A49" s="77" t="s">
+      <c r="A49" s="89" t="s">
         <v>25</v>
       </c>
       <c r="B49" s="24" t="s">
@@ -2156,33 +2156,33 @@
       <c r="C49" s="6">
         <v>65</v>
       </c>
-      <c r="D49" s="92"/>
-      <c r="E49" s="92"/>
+      <c r="D49" s="75"/>
+      <c r="E49" s="75"/>
     </row>
     <row r="50" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A50" s="75"/>
+      <c r="A50" s="90"/>
       <c r="B50" s="23" t="s">
         <v>26</v>
       </c>
       <c r="C50" s="6">
         <v>2</v>
       </c>
-      <c r="D50" s="92"/>
-      <c r="E50" s="92"/>
+      <c r="D50" s="75"/>
+      <c r="E50" s="75"/>
     </row>
     <row r="51" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A51" s="75"/>
+      <c r="A51" s="90"/>
       <c r="B51" s="12" t="s">
         <v>110</v>
       </c>
       <c r="C51" s="7">
         <v>11</v>
       </c>
-      <c r="D51" s="91"/>
-      <c r="E51" s="91"/>
+      <c r="D51" s="74"/>
+      <c r="E51" s="74"/>
     </row>
     <row r="52" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A52" s="83" t="s">
+      <c r="A52" s="93" t="s">
         <v>27</v>
       </c>
       <c r="B52" s="29" t="s">
@@ -2191,19 +2191,19 @@
       <c r="C52" s="7">
         <v>30</v>
       </c>
-      <c r="D52" s="91"/>
-      <c r="E52" s="91"/>
+      <c r="D52" s="74"/>
+      <c r="E52" s="74"/>
     </row>
     <row r="53" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A53" s="84"/>
+      <c r="A53" s="94"/>
       <c r="B53" s="22" t="s">
         <v>101</v>
       </c>
       <c r="C53" s="7">
         <v>95</v>
       </c>
-      <c r="D53" s="91"/>
-      <c r="E53" s="91"/>
+      <c r="D53" s="74"/>
+      <c r="E53" s="74"/>
     </row>
     <row r="54" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A54" s="1" t="s">
@@ -2215,11 +2215,11 @@
       <c r="C54" s="6">
         <v>9</v>
       </c>
-      <c r="D54" s="92"/>
-      <c r="E54" s="92"/>
+      <c r="D54" s="75"/>
+      <c r="E54" s="75"/>
     </row>
     <row r="55" spans="1:5" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A55" s="77" t="s">
+      <c r="A55" s="89" t="s">
         <v>29</v>
       </c>
       <c r="B55" s="27" t="s">
@@ -2228,19 +2228,19 @@
       <c r="C55" s="6">
         <v>7</v>
       </c>
-      <c r="D55" s="92"/>
-      <c r="E55" s="92"/>
+      <c r="D55" s="75"/>
+      <c r="E55" s="75"/>
     </row>
     <row r="56" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A56" s="75"/>
+      <c r="A56" s="90"/>
       <c r="B56" s="9" t="s">
         <v>105</v>
       </c>
       <c r="C56" s="6">
         <v>3</v>
       </c>
-      <c r="D56" s="92"/>
-      <c r="E56" s="92"/>
+      <c r="D56" s="75"/>
+      <c r="E56" s="75"/>
     </row>
     <row r="57" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A57" s="1" t="s">
@@ -2252,8 +2252,8 @@
       <c r="C57" s="6">
         <v>23</v>
       </c>
-      <c r="D57" s="92"/>
-      <c r="E57" s="92"/>
+      <c r="D57" s="75"/>
+      <c r="E57" s="75"/>
     </row>
     <row r="58" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A58" s="1" t="s">
@@ -2265,11 +2265,11 @@
       <c r="C58" s="6">
         <v>4</v>
       </c>
-      <c r="D58" s="92"/>
-      <c r="E58" s="92"/>
+      <c r="D58" s="75"/>
+      <c r="E58" s="75"/>
     </row>
     <row r="59" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A59" s="77" t="s">
+      <c r="A59" s="89" t="s">
         <v>32</v>
       </c>
       <c r="B59" s="28" t="s">
@@ -2278,41 +2278,41 @@
       <c r="C59" s="6">
         <v>35</v>
       </c>
-      <c r="D59" s="92"/>
-      <c r="E59" s="92"/>
+      <c r="D59" s="75"/>
+      <c r="E59" s="75"/>
     </row>
     <row r="60" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A60" s="75"/>
+      <c r="A60" s="90"/>
       <c r="B60" s="24" t="s">
         <v>104</v>
       </c>
       <c r="C60" s="6">
         <v>28</v>
       </c>
-      <c r="D60" s="92"/>
-      <c r="E60" s="92"/>
+      <c r="D60" s="75"/>
+      <c r="E60" s="75"/>
     </row>
     <row r="61" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A61" s="75"/>
+      <c r="A61" s="90"/>
       <c r="B61" s="32" t="s">
         <v>133</v>
       </c>
       <c r="C61" s="6">
         <v>2</v>
       </c>
-      <c r="D61" s="92"/>
-      <c r="E61" s="92"/>
+      <c r="D61" s="75"/>
+      <c r="E61" s="75"/>
     </row>
     <row r="62" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A62" s="75"/>
+      <c r="A62" s="90"/>
       <c r="B62" s="13" t="s">
         <v>106</v>
       </c>
       <c r="C62" s="6">
         <v>1</v>
       </c>
-      <c r="D62" s="92"/>
-      <c r="E62" s="92"/>
+      <c r="D62" s="75"/>
+      <c r="E62" s="75"/>
     </row>
     <row r="63" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A63" s="1" t="s">
@@ -2324,8 +2324,8 @@
       <c r="C63" s="6">
         <v>49</v>
       </c>
-      <c r="D63" s="92"/>
-      <c r="E63" s="92"/>
+      <c r="D63" s="75"/>
+      <c r="E63" s="75"/>
     </row>
     <row r="64" spans="1:5" ht="49.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A64" s="1" t="s">
@@ -2335,33 +2335,33 @@
         <v>35</v>
       </c>
       <c r="C64" s="6"/>
-      <c r="D64" s="92"/>
-      <c r="E64" s="92"/>
+      <c r="D64" s="75"/>
+      <c r="E64" s="75"/>
     </row>
     <row r="65" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A65" s="77" t="s">
+      <c r="A65" s="89" t="s">
         <v>36</v>
       </c>
       <c r="B65" s="33" t="s">
         <v>139</v>
       </c>
-      <c r="C65" s="76">
-        <v>1</v>
-      </c>
-      <c r="D65" s="92"/>
-      <c r="E65" s="92"/>
+      <c r="C65" s="104">
+        <v>1</v>
+      </c>
+      <c r="D65" s="75"/>
+      <c r="E65" s="75"/>
     </row>
     <row r="66" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A66" s="75"/>
+      <c r="A66" s="90"/>
       <c r="B66" s="23" t="s">
         <v>148</v>
       </c>
-      <c r="C66" s="76"/>
-      <c r="D66" s="92"/>
-      <c r="E66" s="92"/>
+      <c r="C66" s="104"/>
+      <c r="D66" s="75"/>
+      <c r="E66" s="75"/>
     </row>
     <row r="67" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A67" s="77" t="s">
+      <c r="A67" s="89" t="s">
         <v>37</v>
       </c>
       <c r="B67" s="32" t="s">
@@ -2370,41 +2370,41 @@
       <c r="C67" s="6">
         <v>3</v>
       </c>
-      <c r="D67" s="92"/>
-      <c r="E67" s="92"/>
+      <c r="D67" s="75"/>
+      <c r="E67" s="75"/>
     </row>
     <row r="68" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A68" s="75"/>
+      <c r="A68" s="90"/>
       <c r="B68" s="22" t="s">
         <v>101</v>
       </c>
       <c r="C68" s="6">
         <v>3</v>
       </c>
-      <c r="D68" s="92"/>
-      <c r="E68" s="92"/>
+      <c r="D68" s="75"/>
+      <c r="E68" s="75"/>
     </row>
     <row r="69" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A69" s="75"/>
+      <c r="A69" s="90"/>
       <c r="B69" s="34" t="s">
         <v>117</v>
       </c>
       <c r="C69" s="6">
         <v>3</v>
       </c>
-      <c r="D69" s="92"/>
-      <c r="E69" s="92"/>
+      <c r="D69" s="75"/>
+      <c r="E69" s="75"/>
     </row>
     <row r="70" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A70" s="75"/>
+      <c r="A70" s="90"/>
       <c r="B70" s="33" t="s">
         <v>38</v>
       </c>
       <c r="C70" s="6">
         <v>3</v>
       </c>
-      <c r="D70" s="92"/>
-      <c r="E70" s="92"/>
+      <c r="D70" s="75"/>
+      <c r="E70" s="75"/>
     </row>
     <row r="71" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A71" s="1" t="s">
@@ -2416,8 +2416,8 @@
       <c r="C71" s="6">
         <v>20</v>
       </c>
-      <c r="D71" s="92"/>
-      <c r="E71" s="92"/>
+      <c r="D71" s="75"/>
+      <c r="E71" s="75"/>
     </row>
     <row r="72" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A72" s="3"/>
@@ -2427,8 +2427,8 @@
       <c r="C72" s="7">
         <v>1</v>
       </c>
-      <c r="D72" s="91"/>
-      <c r="E72" s="91"/>
+      <c r="D72" s="74"/>
+      <c r="E72" s="74"/>
     </row>
     <row r="73" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A73" s="3"/>
@@ -2438,8 +2438,8 @@
       <c r="C73" s="6">
         <v>16</v>
       </c>
-      <c r="D73" s="92"/>
-      <c r="E73" s="92"/>
+      <c r="D73" s="75"/>
+      <c r="E73" s="75"/>
     </row>
     <row r="74" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A74" s="3"/>
@@ -2449,8 +2449,8 @@
       <c r="C74" s="7">
         <v>2</v>
       </c>
-      <c r="D74" s="91"/>
-      <c r="E74" s="91"/>
+      <c r="D74" s="74"/>
+      <c r="E74" s="74"/>
     </row>
     <row r="75" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A75" s="3"/>
@@ -2458,8 +2458,8 @@
         <v>149</v>
       </c>
       <c r="C75" s="10"/>
-      <c r="D75" s="94"/>
-      <c r="E75" s="94"/>
+      <c r="D75" s="77"/>
+      <c r="E75" s="77"/>
     </row>
     <row r="76" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A76" s="63" t="s">
@@ -2469,8 +2469,8 @@
         <v>99</v>
       </c>
       <c r="C76" s="10"/>
-      <c r="D76" s="94"/>
-      <c r="E76" s="94"/>
+      <c r="D76" s="77"/>
+      <c r="E76" s="77"/>
     </row>
     <row r="77" spans="1:5" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A77" s="3"/>
@@ -2480,11 +2480,11 @@
       <c r="C77" s="6" t="s">
         <v>162</v>
       </c>
-      <c r="D77" s="92"/>
-      <c r="E77" s="92"/>
+      <c r="D77" s="75"/>
+      <c r="E77" s="75"/>
     </row>
     <row r="78" spans="1:5" ht="27" x14ac:dyDescent="0.2">
-      <c r="A78" s="77" t="s">
+      <c r="A78" s="89" t="s">
         <v>39</v>
       </c>
       <c r="B78" s="23" t="s">
@@ -2493,33 +2493,33 @@
       <c r="C78" s="6" t="s">
         <v>163</v>
       </c>
-      <c r="D78" s="92"/>
-      <c r="E78" s="92"/>
+      <c r="D78" s="75"/>
+      <c r="E78" s="75"/>
     </row>
     <row r="79" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A79" s="75"/>
+      <c r="A79" s="90"/>
       <c r="B79" s="13" t="s">
         <v>106</v>
       </c>
       <c r="C79" s="6">
         <v>5</v>
       </c>
-      <c r="D79" s="92"/>
-      <c r="E79" s="92"/>
+      <c r="D79" s="75"/>
+      <c r="E79" s="75"/>
     </row>
     <row r="80" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A80" s="75"/>
+      <c r="A80" s="90"/>
       <c r="B80" s="27" t="s">
         <v>103</v>
       </c>
       <c r="C80" s="6">
         <v>4</v>
       </c>
-      <c r="D80" s="92"/>
-      <c r="E80" s="92"/>
+      <c r="D80" s="75"/>
+      <c r="E80" s="75"/>
     </row>
     <row r="81" spans="1:5" ht="48.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A81" s="77" t="s">
+      <c r="A81" s="89" t="s">
         <v>40</v>
       </c>
       <c r="B81" s="15" t="s">
@@ -2528,33 +2528,33 @@
       <c r="C81" s="6">
         <v>5</v>
       </c>
-      <c r="D81" s="92"/>
-      <c r="E81" s="92"/>
+      <c r="D81" s="75"/>
+      <c r="E81" s="75"/>
     </row>
     <row r="82" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A82" s="75"/>
+      <c r="A82" s="90"/>
       <c r="B82" s="16" t="s">
         <v>105</v>
       </c>
       <c r="C82" s="6">
         <v>4</v>
       </c>
-      <c r="D82" s="92"/>
-      <c r="E82" s="92"/>
+      <c r="D82" s="75"/>
+      <c r="E82" s="75"/>
     </row>
     <row r="83" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A83" s="75"/>
+      <c r="A83" s="90"/>
       <c r="B83" s="39" t="s">
         <v>103</v>
       </c>
       <c r="C83" s="6">
         <v>5</v>
       </c>
-      <c r="D83" s="92"/>
-      <c r="E83" s="92"/>
+      <c r="D83" s="75"/>
+      <c r="E83" s="75"/>
     </row>
     <row r="84" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A84" s="77" t="s">
+      <c r="A84" s="89" t="s">
         <v>41</v>
       </c>
       <c r="B84" s="12" t="s">
@@ -2563,42 +2563,42 @@
       <c r="C84" s="6">
         <v>7</v>
       </c>
-      <c r="D84" s="92"/>
-      <c r="E84" s="92"/>
+      <c r="D84" s="75"/>
+      <c r="E84" s="75"/>
     </row>
     <row r="85" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A85" s="75"/>
+      <c r="A85" s="90"/>
       <c r="B85" s="27" t="s">
         <v>131</v>
       </c>
       <c r="C85" s="6">
         <v>2</v>
       </c>
-      <c r="D85" s="92"/>
-      <c r="E85" s="92"/>
+      <c r="D85" s="75"/>
+      <c r="E85" s="75"/>
     </row>
     <row r="86" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A86" s="75"/>
+      <c r="A86" s="90"/>
       <c r="B86" s="25" t="s">
         <v>109</v>
       </c>
       <c r="C86" s="6">
         <v>2</v>
       </c>
-      <c r="D86" s="92"/>
-      <c r="E86" s="92"/>
+      <c r="D86" s="75"/>
+      <c r="E86" s="75"/>
     </row>
     <row r="87" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A87" s="75"/>
+      <c r="A87" s="90"/>
       <c r="B87" s="23" t="s">
         <v>43</v>
       </c>
       <c r="C87" s="6"/>
-      <c r="D87" s="92"/>
-      <c r="E87" s="92"/>
+      <c r="D87" s="75"/>
+      <c r="E87" s="75"/>
     </row>
     <row r="88" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A88" s="77" t="s">
+      <c r="A88" s="89" t="s">
         <v>44</v>
       </c>
       <c r="B88" s="40" t="s">
@@ -2607,83 +2607,83 @@
       <c r="C88" s="6">
         <v>6</v>
       </c>
-      <c r="D88" s="92"/>
-      <c r="E88" s="92"/>
+      <c r="D88" s="75"/>
+      <c r="E88" s="75"/>
     </row>
     <row r="89" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A89" s="75"/>
+      <c r="A89" s="90"/>
       <c r="B89" s="17" t="s">
         <v>115</v>
       </c>
       <c r="C89" s="6">
         <v>4</v>
       </c>
-      <c r="D89" s="92"/>
-      <c r="E89" s="92"/>
+      <c r="D89" s="75"/>
+      <c r="E89" s="75"/>
     </row>
     <row r="90" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A90" s="75"/>
+      <c r="A90" s="90"/>
       <c r="B90" s="28" t="s">
         <v>111</v>
       </c>
       <c r="C90" s="6">
         <v>3</v>
       </c>
-      <c r="D90" s="92"/>
-      <c r="E90" s="92"/>
+      <c r="D90" s="75"/>
+      <c r="E90" s="75"/>
     </row>
     <row r="91" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A91" s="75"/>
+      <c r="A91" s="90"/>
       <c r="B91" s="22" t="s">
         <v>146</v>
       </c>
       <c r="C91" s="6">
         <v>3</v>
       </c>
-      <c r="D91" s="92"/>
-      <c r="E91" s="92"/>
+      <c r="D91" s="75"/>
+      <c r="E91" s="75"/>
     </row>
     <row r="92" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A92" s="75"/>
+      <c r="A92" s="90"/>
       <c r="B92" s="18" t="s">
         <v>45</v>
       </c>
       <c r="C92" s="6">
         <v>5</v>
       </c>
-      <c r="D92" s="92"/>
-      <c r="E92" s="92"/>
+      <c r="D92" s="75"/>
+      <c r="E92" s="75"/>
     </row>
     <row r="93" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A93" s="75"/>
+      <c r="A93" s="90"/>
       <c r="B93" s="27" t="s">
         <v>103</v>
       </c>
       <c r="C93" s="6">
         <v>4</v>
       </c>
-      <c r="D93" s="92"/>
-      <c r="E93" s="92"/>
+      <c r="D93" s="75"/>
+      <c r="E93" s="75"/>
     </row>
     <row r="94" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A94" s="75"/>
+      <c r="A94" s="90"/>
       <c r="B94" s="32" t="s">
         <v>108</v>
       </c>
       <c r="C94" s="6">
         <v>1</v>
       </c>
-      <c r="D94" s="92"/>
-      <c r="E94" s="92"/>
+      <c r="D94" s="75"/>
+      <c r="E94" s="75"/>
     </row>
     <row r="95" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A95" s="75"/>
+      <c r="A95" s="90"/>
       <c r="B95" s="23" t="s">
         <v>123</v>
       </c>
       <c r="C95" s="6"/>
-      <c r="D95" s="92"/>
-      <c r="E95" s="92"/>
+      <c r="D95" s="75"/>
+      <c r="E95" s="75"/>
     </row>
     <row r="96" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A96" s="1" t="s">
@@ -2691,11 +2691,11 @@
       </c>
       <c r="B96" s="23"/>
       <c r="C96" s="6"/>
-      <c r="D96" s="92"/>
-      <c r="E96" s="92"/>
+      <c r="D96" s="75"/>
+      <c r="E96" s="75"/>
     </row>
     <row r="97" spans="1:5" ht="33.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A97" s="77" t="s">
+      <c r="A97" s="89" t="s">
         <v>48</v>
       </c>
       <c r="B97" s="15" t="s">
@@ -2704,33 +2704,33 @@
       <c r="C97" s="7">
         <v>6</v>
       </c>
-      <c r="D97" s="91"/>
-      <c r="E97" s="91"/>
+      <c r="D97" s="74"/>
+      <c r="E97" s="74"/>
     </row>
     <row r="98" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A98" s="75"/>
+      <c r="A98" s="90"/>
       <c r="B98" s="16" t="s">
         <v>105</v>
       </c>
       <c r="C98" s="7">
         <v>5</v>
       </c>
-      <c r="D98" s="91"/>
-      <c r="E98" s="91"/>
+      <c r="D98" s="74"/>
+      <c r="E98" s="74"/>
     </row>
     <row r="99" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A99" s="75"/>
+      <c r="A99" s="90"/>
       <c r="B99" s="39" t="s">
         <v>103</v>
       </c>
       <c r="C99" s="7">
         <v>2</v>
       </c>
-      <c r="D99" s="91"/>
-      <c r="E99" s="91"/>
+      <c r="D99" s="74"/>
+      <c r="E99" s="74"/>
     </row>
     <row r="100" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A100" s="77" t="s">
+      <c r="A100" s="89" t="s">
         <v>49</v>
       </c>
       <c r="B100" s="15" t="s">
@@ -2739,55 +2739,55 @@
       <c r="C100" s="7">
         <v>16</v>
       </c>
-      <c r="D100" s="91"/>
-      <c r="E100" s="91"/>
+      <c r="D100" s="74"/>
+      <c r="E100" s="74"/>
     </row>
     <row r="101" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A101" s="75"/>
+      <c r="A101" s="90"/>
       <c r="B101" s="16" t="s">
         <v>105</v>
       </c>
       <c r="C101" s="7">
         <v>6</v>
       </c>
-      <c r="D101" s="91"/>
-      <c r="E101" s="91"/>
+      <c r="D101" s="74"/>
+      <c r="E101" s="74"/>
     </row>
     <row r="102" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A102" s="75"/>
+      <c r="A102" s="90"/>
       <c r="B102" s="11" t="s">
         <v>125</v>
       </c>
       <c r="C102" s="7">
         <v>1</v>
       </c>
-      <c r="D102" s="91"/>
-      <c r="E102" s="91"/>
+      <c r="D102" s="74"/>
+      <c r="E102" s="74"/>
     </row>
     <row r="103" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A103" s="75"/>
+      <c r="A103" s="90"/>
       <c r="B103" s="41" t="s">
         <v>50</v>
       </c>
       <c r="C103" s="7">
         <v>1</v>
       </c>
-      <c r="D103" s="91"/>
-      <c r="E103" s="91"/>
+      <c r="D103" s="74"/>
+      <c r="E103" s="74"/>
     </row>
     <row r="104" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A104" s="75"/>
+      <c r="A104" s="90"/>
       <c r="B104" s="39" t="s">
         <v>103</v>
       </c>
       <c r="C104" s="7">
         <v>11</v>
       </c>
-      <c r="D104" s="91"/>
-      <c r="E104" s="91"/>
+      <c r="D104" s="74"/>
+      <c r="E104" s="74"/>
     </row>
     <row r="105" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A105" s="77" t="s">
+      <c r="A105" s="89" t="s">
         <v>51</v>
       </c>
       <c r="B105" s="36" t="s">
@@ -2796,225 +2796,225 @@
       <c r="C105" s="8">
         <v>26</v>
       </c>
-      <c r="D105" s="95"/>
-      <c r="E105" s="95"/>
+      <c r="D105" s="78"/>
+      <c r="E105" s="78"/>
     </row>
     <row r="106" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A106" s="75"/>
+      <c r="A106" s="90"/>
       <c r="B106" s="23" t="s">
         <v>151</v>
       </c>
       <c r="C106" s="6">
         <v>11</v>
       </c>
-      <c r="D106" s="92"/>
-      <c r="E106" s="92"/>
+      <c r="D106" s="75"/>
+      <c r="E106" s="75"/>
     </row>
     <row r="107" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A107" s="75"/>
+      <c r="A107" s="90"/>
       <c r="B107" s="34" t="s">
         <v>142</v>
       </c>
       <c r="C107" s="6">
         <v>13</v>
       </c>
-      <c r="D107" s="92"/>
-      <c r="E107" s="92"/>
+      <c r="D107" s="75"/>
+      <c r="E107" s="75"/>
     </row>
     <row r="108" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A108" s="75"/>
+      <c r="A108" s="90"/>
       <c r="B108" s="42" t="s">
         <v>116</v>
       </c>
       <c r="C108" s="6">
         <v>4</v>
       </c>
-      <c r="D108" s="92"/>
-      <c r="E108" s="92"/>
+      <c r="D108" s="75"/>
+      <c r="E108" s="75"/>
     </row>
     <row r="109" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A109" s="75"/>
+      <c r="A109" s="90"/>
       <c r="B109" s="24" t="s">
         <v>104</v>
       </c>
       <c r="C109" s="6">
         <v>2</v>
       </c>
-      <c r="D109" s="92"/>
-      <c r="E109" s="92"/>
+      <c r="D109" s="75"/>
+      <c r="E109" s="75"/>
     </row>
     <row r="110" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A110" s="75"/>
+      <c r="A110" s="90"/>
       <c r="B110" s="32" t="s">
         <v>108</v>
       </c>
       <c r="C110" s="6">
         <v>12</v>
       </c>
-      <c r="D110" s="92"/>
-      <c r="E110" s="92"/>
+      <c r="D110" s="75"/>
+      <c r="E110" s="75"/>
     </row>
     <row r="111" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A111" s="75"/>
+      <c r="A111" s="90"/>
       <c r="B111" s="22" t="s">
         <v>101</v>
       </c>
       <c r="C111" s="6">
         <v>1</v>
       </c>
-      <c r="D111" s="92"/>
-      <c r="E111" s="92"/>
+      <c r="D111" s="75"/>
+      <c r="E111" s="75"/>
     </row>
     <row r="112" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A112" s="75"/>
+      <c r="A112" s="90"/>
       <c r="B112" s="41" t="s">
         <v>153</v>
       </c>
       <c r="C112" s="6">
         <v>1</v>
       </c>
-      <c r="D112" s="92"/>
-      <c r="E112" s="92"/>
+      <c r="D112" s="75"/>
+      <c r="E112" s="75"/>
     </row>
     <row r="113" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A113" s="75"/>
+      <c r="A113" s="90"/>
       <c r="B113" s="19" t="s">
         <v>118</v>
       </c>
       <c r="C113" s="6">
         <v>7</v>
       </c>
-      <c r="D113" s="92"/>
-      <c r="E113" s="92"/>
+      <c r="D113" s="75"/>
+      <c r="E113" s="75"/>
     </row>
     <row r="114" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A114" s="75"/>
+      <c r="A114" s="90"/>
       <c r="B114" s="16" t="s">
         <v>105</v>
       </c>
       <c r="C114" s="6">
         <v>2</v>
       </c>
-      <c r="D114" s="92"/>
-      <c r="E114" s="92"/>
+      <c r="D114" s="75"/>
+      <c r="E114" s="75"/>
     </row>
     <row r="115" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A115" s="75"/>
+      <c r="A115" s="90"/>
       <c r="B115" s="41" t="s">
         <v>154</v>
       </c>
       <c r="C115" s="6">
         <v>4</v>
       </c>
-      <c r="D115" s="92"/>
-      <c r="E115" s="92"/>
+      <c r="D115" s="75"/>
+      <c r="E115" s="75"/>
     </row>
     <row r="116" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A116" s="75"/>
+      <c r="A116" s="90"/>
       <c r="B116" s="41" t="s">
         <v>26</v>
       </c>
       <c r="C116" s="6">
         <v>1</v>
       </c>
-      <c r="D116" s="92"/>
-      <c r="E116" s="92"/>
+      <c r="D116" s="75"/>
+      <c r="E116" s="75"/>
     </row>
     <row r="117" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A117" s="75"/>
+      <c r="A117" s="90"/>
       <c r="B117" s="41" t="s">
         <v>88</v>
       </c>
       <c r="C117" s="6">
         <v>1</v>
       </c>
-      <c r="D117" s="92"/>
-      <c r="E117" s="92"/>
+      <c r="D117" s="75"/>
+      <c r="E117" s="75"/>
     </row>
     <row r="118" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A118" s="75"/>
+      <c r="A118" s="90"/>
       <c r="B118" s="41" t="s">
         <v>155</v>
       </c>
       <c r="C118" s="6">
         <v>1</v>
       </c>
-      <c r="D118" s="92"/>
-      <c r="E118" s="92"/>
+      <c r="D118" s="75"/>
+      <c r="E118" s="75"/>
     </row>
     <row r="119" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A119" s="75"/>
+      <c r="A119" s="90"/>
       <c r="B119" s="41" t="s">
         <v>156</v>
       </c>
       <c r="C119" s="6">
         <v>1</v>
       </c>
-      <c r="D119" s="92"/>
-      <c r="E119" s="92"/>
+      <c r="D119" s="75"/>
+      <c r="E119" s="75"/>
     </row>
     <row r="120" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A120" s="75"/>
+      <c r="A120" s="90"/>
       <c r="B120" s="41" t="s">
         <v>157</v>
       </c>
       <c r="C120" s="6">
         <v>1</v>
       </c>
-      <c r="D120" s="92"/>
-      <c r="E120" s="92"/>
+      <c r="D120" s="75"/>
+      <c r="E120" s="75"/>
     </row>
     <row r="121" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A121" s="75"/>
+      <c r="A121" s="90"/>
       <c r="B121" s="41" t="s">
         <v>76</v>
       </c>
       <c r="C121" s="6">
         <v>1</v>
       </c>
-      <c r="D121" s="92"/>
-      <c r="E121" s="92"/>
+      <c r="D121" s="75"/>
+      <c r="E121" s="75"/>
     </row>
     <row r="122" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A122" s="75"/>
+      <c r="A122" s="90"/>
       <c r="B122" s="43" t="s">
         <v>114</v>
       </c>
       <c r="C122" s="6">
         <v>1</v>
       </c>
-      <c r="D122" s="92"/>
-      <c r="E122" s="92"/>
+      <c r="D122" s="75"/>
+      <c r="E122" s="75"/>
     </row>
     <row r="123" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A123" s="75"/>
+      <c r="A123" s="90"/>
       <c r="B123" s="23" t="s">
         <v>97</v>
       </c>
       <c r="C123" s="6"/>
-      <c r="D123" s="92"/>
-      <c r="E123" s="92"/>
+      <c r="D123" s="75"/>
+      <c r="E123" s="75"/>
     </row>
     <row r="124" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A124" s="75"/>
+      <c r="A124" s="90"/>
       <c r="B124" s="23" t="s">
         <v>121</v>
       </c>
       <c r="C124" s="6"/>
-      <c r="D124" s="92"/>
-      <c r="E124" s="92"/>
+      <c r="D124" s="75"/>
+      <c r="E124" s="75"/>
     </row>
     <row r="125" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A125" s="75"/>
+      <c r="A125" s="90"/>
       <c r="B125" s="53" t="s">
         <v>46</v>
       </c>
       <c r="C125" s="54"/>
-      <c r="D125" s="96"/>
-      <c r="E125" s="96"/>
+      <c r="D125" s="79"/>
+      <c r="E125" s="79"/>
     </row>
     <row r="126" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A126" s="77" t="s">
+      <c r="A126" s="89" t="s">
         <v>52</v>
       </c>
       <c r="B126" s="29" t="s">
@@ -3023,139 +3023,139 @@
       <c r="C126" s="6">
         <v>37</v>
       </c>
-      <c r="D126" s="92"/>
-      <c r="E126" s="92"/>
+      <c r="D126" s="75"/>
+      <c r="E126" s="75"/>
     </row>
     <row r="127" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A127" s="75"/>
+      <c r="A127" s="90"/>
       <c r="B127" s="41" t="s">
         <v>53</v>
       </c>
       <c r="C127" s="6">
         <v>10</v>
       </c>
-      <c r="D127" s="92"/>
-      <c r="E127" s="92"/>
+      <c r="D127" s="75"/>
+      <c r="E127" s="75"/>
     </row>
     <row r="128" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A128" s="75"/>
+      <c r="A128" s="90"/>
       <c r="B128" s="44" t="s">
         <v>113</v>
       </c>
       <c r="C128" s="6">
         <v>5</v>
       </c>
-      <c r="D128" s="92"/>
-      <c r="E128" s="92"/>
+      <c r="D128" s="75"/>
+      <c r="E128" s="75"/>
     </row>
     <row r="129" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A129" s="75"/>
+      <c r="A129" s="90"/>
       <c r="B129" s="40" t="s">
         <v>102</v>
       </c>
       <c r="C129" s="6">
         <v>2</v>
       </c>
-      <c r="D129" s="92"/>
-      <c r="E129" s="92"/>
+      <c r="D129" s="75"/>
+      <c r="E129" s="75"/>
     </row>
     <row r="130" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A130" s="75"/>
+      <c r="A130" s="90"/>
       <c r="B130" s="27" t="s">
         <v>103</v>
       </c>
       <c r="C130" s="6">
         <v>1</v>
       </c>
-      <c r="D130" s="92"/>
-      <c r="E130" s="92"/>
+      <c r="D130" s="75"/>
+      <c r="E130" s="75"/>
     </row>
     <row r="131" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A131" s="75"/>
+      <c r="A131" s="90"/>
       <c r="B131" s="9" t="s">
         <v>105</v>
       </c>
       <c r="C131" s="6">
         <v>2</v>
       </c>
-      <c r="D131" s="92"/>
-      <c r="E131" s="92"/>
+      <c r="D131" s="75"/>
+      <c r="E131" s="75"/>
     </row>
     <row r="132" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A132" s="75"/>
+      <c r="A132" s="90"/>
       <c r="B132" s="22" t="s">
         <v>101</v>
       </c>
       <c r="C132" s="6">
         <v>1</v>
       </c>
-      <c r="D132" s="92"/>
-      <c r="E132" s="92"/>
+      <c r="D132" s="75"/>
+      <c r="E132" s="75"/>
     </row>
     <row r="133" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A133" s="75"/>
+      <c r="A133" s="90"/>
       <c r="B133" s="17" t="s">
         <v>115</v>
       </c>
       <c r="C133" s="6">
         <v>4</v>
       </c>
-      <c r="D133" s="92"/>
-      <c r="E133" s="92"/>
+      <c r="D133" s="75"/>
+      <c r="E133" s="75"/>
     </row>
     <row r="134" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A134" s="75"/>
+      <c r="A134" s="90"/>
       <c r="B134" s="41" t="s">
         <v>54</v>
       </c>
       <c r="C134" s="6">
         <v>5</v>
       </c>
-      <c r="D134" s="92"/>
-      <c r="E134" s="92"/>
+      <c r="D134" s="75"/>
+      <c r="E134" s="75"/>
     </row>
     <row r="135" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A135" s="75"/>
+      <c r="A135" s="90"/>
       <c r="B135" s="45" t="s">
         <v>112</v>
       </c>
       <c r="C135" s="6">
         <v>2</v>
       </c>
-      <c r="D135" s="92"/>
-      <c r="E135" s="92"/>
+      <c r="D135" s="75"/>
+      <c r="E135" s="75"/>
     </row>
     <row r="136" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A136" s="75"/>
+      <c r="A136" s="90"/>
       <c r="B136" s="18" t="s">
         <v>118</v>
       </c>
       <c r="C136" s="6">
         <v>1</v>
       </c>
-      <c r="D136" s="92"/>
-      <c r="E136" s="92"/>
+      <c r="D136" s="75"/>
+      <c r="E136" s="75"/>
     </row>
     <row r="137" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A137" s="75"/>
+      <c r="A137" s="90"/>
       <c r="B137" s="23" t="s">
         <v>64</v>
       </c>
       <c r="C137" s="6"/>
-      <c r="D137" s="92"/>
-      <c r="E137" s="92"/>
+      <c r="D137" s="75"/>
+      <c r="E137" s="75"/>
     </row>
     <row r="138" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A138" s="75"/>
+      <c r="A138" s="90"/>
       <c r="B138" s="53" t="s">
         <v>46</v>
       </c>
       <c r="C138" s="64"/>
-      <c r="D138" s="97"/>
-      <c r="E138" s="97"/>
+      <c r="D138" s="80"/>
+      <c r="E138" s="80"/>
     </row>
     <row r="139" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A139" s="77" t="s">
+      <c r="A139" s="89" t="s">
         <v>56</v>
       </c>
       <c r="B139" s="42" t="s">
@@ -3164,136 +3164,136 @@
       <c r="C139" s="6">
         <v>6</v>
       </c>
-      <c r="D139" s="92"/>
-      <c r="E139" s="92"/>
+      <c r="D139" s="75"/>
+      <c r="E139" s="75"/>
     </row>
     <row r="140" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A140" s="75"/>
+      <c r="A140" s="90"/>
       <c r="B140" s="41" t="s">
         <v>93</v>
       </c>
       <c r="C140" s="6">
         <v>2</v>
       </c>
-      <c r="D140" s="92"/>
-      <c r="E140" s="92"/>
+      <c r="D140" s="75"/>
+      <c r="E140" s="75"/>
     </row>
     <row r="141" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A141" s="75"/>
+      <c r="A141" s="90"/>
       <c r="B141" s="27" t="s">
         <v>132</v>
       </c>
       <c r="C141" s="6">
         <v>6</v>
       </c>
-      <c r="D141" s="92"/>
-      <c r="E141" s="92"/>
+      <c r="D141" s="75"/>
+      <c r="E141" s="75"/>
     </row>
     <row r="142" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A142" s="75"/>
+      <c r="A142" s="90"/>
       <c r="B142" s="41" t="s">
         <v>57</v>
       </c>
       <c r="C142" s="6">
         <v>8</v>
       </c>
-      <c r="D142" s="92"/>
-      <c r="E142" s="92"/>
+      <c r="D142" s="75"/>
+      <c r="E142" s="75"/>
     </row>
     <row r="143" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A143" s="75"/>
+      <c r="A143" s="90"/>
       <c r="B143" s="40" t="s">
         <v>102</v>
       </c>
       <c r="C143" s="6">
         <v>2</v>
       </c>
-      <c r="D143" s="92"/>
-      <c r="E143" s="92"/>
+      <c r="D143" s="75"/>
+      <c r="E143" s="75"/>
     </row>
     <row r="144" spans="1:5" ht="31.5" x14ac:dyDescent="0.2">
-      <c r="A144" s="75"/>
+      <c r="A144" s="90"/>
       <c r="B144" s="41" t="s">
         <v>58</v>
       </c>
       <c r="C144" s="6">
         <v>6</v>
       </c>
-      <c r="D144" s="92"/>
-      <c r="E144" s="92"/>
+      <c r="D144" s="75"/>
+      <c r="E144" s="75"/>
     </row>
     <row r="145" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A145" s="75"/>
+      <c r="A145" s="90"/>
       <c r="B145" s="11" t="s">
         <v>125</v>
       </c>
       <c r="C145" s="6">
         <v>3</v>
       </c>
-      <c r="D145" s="92"/>
-      <c r="E145" s="92"/>
+      <c r="D145" s="75"/>
+      <c r="E145" s="75"/>
     </row>
     <row r="146" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A146" s="75"/>
+      <c r="A146" s="90"/>
       <c r="B146" s="17" t="s">
         <v>115</v>
       </c>
       <c r="C146" s="6">
         <v>4</v>
       </c>
-      <c r="D146" s="92"/>
-      <c r="E146" s="92"/>
+      <c r="D146" s="75"/>
+      <c r="E146" s="75"/>
     </row>
     <row r="147" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A147" s="75"/>
-      <c r="B147" s="73" t="s">
+      <c r="A147" s="90"/>
+      <c r="B147" s="97" t="s">
         <v>59</v>
       </c>
-      <c r="C147" s="75"/>
-      <c r="D147" s="98"/>
-      <c r="E147" s="98"/>
+      <c r="C147" s="90"/>
+      <c r="D147" s="81"/>
+      <c r="E147" s="81"/>
     </row>
     <row r="148" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A148" s="75"/>
+      <c r="A148" s="90"/>
       <c r="B148" s="22" t="s">
         <v>101</v>
       </c>
       <c r="C148" s="6">
         <v>1</v>
       </c>
-      <c r="D148" s="92"/>
-      <c r="E148" s="92"/>
+      <c r="D148" s="75"/>
+      <c r="E148" s="75"/>
     </row>
     <row r="149" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A149" s="75"/>
+      <c r="A149" s="90"/>
       <c r="B149" s="23" t="s">
         <v>158</v>
       </c>
       <c r="C149" s="6">
         <v>1</v>
       </c>
-      <c r="D149" s="92"/>
-      <c r="E149" s="92"/>
+      <c r="D149" s="75"/>
+      <c r="E149" s="75"/>
     </row>
     <row r="150" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A150" s="75"/>
+      <c r="A150" s="90"/>
       <c r="B150" s="23" t="s">
         <v>60</v>
       </c>
       <c r="C150" s="6">
         <v>5</v>
       </c>
-      <c r="D150" s="92"/>
-      <c r="E150" s="92"/>
+      <c r="D150" s="75"/>
+      <c r="E150" s="75"/>
     </row>
     <row r="151" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A151" s="75"/>
+      <c r="A151" s="90"/>
       <c r="B151" s="53" t="s">
         <v>46</v>
       </c>
       <c r="C151" s="64"/>
-      <c r="D151" s="97"/>
-      <c r="E151" s="97"/>
+      <c r="D151" s="80"/>
+      <c r="E151" s="80"/>
     </row>
     <row r="152" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A152" s="1" t="s">
@@ -3305,8 +3305,8 @@
       <c r="C152" s="6">
         <v>4</v>
       </c>
-      <c r="D152" s="92"/>
-      <c r="E152" s="92"/>
+      <c r="D152" s="75"/>
+      <c r="E152" s="75"/>
     </row>
     <row r="153" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A153" s="3"/>
@@ -3316,11 +3316,11 @@
       <c r="C153" s="6">
         <v>1</v>
       </c>
-      <c r="D153" s="92"/>
-      <c r="E153" s="92"/>
+      <c r="D153" s="75"/>
+      <c r="E153" s="75"/>
     </row>
     <row r="154" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A154" s="77" t="s">
+      <c r="A154" s="89" t="s">
         <v>62</v>
       </c>
       <c r="B154" s="40" t="s">
@@ -3329,106 +3329,106 @@
       <c r="C154" s="6">
         <v>4</v>
       </c>
-      <c r="D154" s="92"/>
-      <c r="E154" s="92"/>
+      <c r="D154" s="75"/>
+      <c r="E154" s="75"/>
     </row>
     <row r="155" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A155" s="75"/>
+      <c r="A155" s="90"/>
       <c r="B155" s="28" t="s">
         <v>145</v>
       </c>
       <c r="C155" s="6">
         <v>1</v>
       </c>
-      <c r="D155" s="92"/>
-      <c r="E155" s="92"/>
+      <c r="D155" s="75"/>
+      <c r="E155" s="75"/>
     </row>
     <row r="156" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A156" s="75"/>
+      <c r="A156" s="90"/>
       <c r="B156" s="27" t="s">
         <v>103</v>
       </c>
       <c r="C156" s="6">
         <v>9</v>
       </c>
-      <c r="D156" s="92"/>
-      <c r="E156" s="92"/>
+      <c r="D156" s="75"/>
+      <c r="E156" s="75"/>
     </row>
     <row r="157" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A157" s="75"/>
+      <c r="A157" s="90"/>
       <c r="B157" s="43" t="s">
         <v>114</v>
       </c>
       <c r="C157" s="6">
         <v>1</v>
       </c>
-      <c r="D157" s="92"/>
-      <c r="E157" s="92"/>
+      <c r="D157" s="75"/>
+      <c r="E157" s="75"/>
     </row>
     <row r="158" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A158" s="75"/>
+      <c r="A158" s="90"/>
       <c r="B158" s="9" t="s">
         <v>105</v>
       </c>
       <c r="C158" s="6">
         <v>11</v>
       </c>
-      <c r="D158" s="92"/>
-      <c r="E158" s="92"/>
+      <c r="D158" s="75"/>
+      <c r="E158" s="75"/>
     </row>
     <row r="159" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A159" s="75"/>
+      <c r="A159" s="90"/>
       <c r="B159" s="41" t="s">
         <v>53</v>
       </c>
       <c r="C159" s="6">
         <v>3</v>
       </c>
-      <c r="D159" s="92"/>
-      <c r="E159" s="92"/>
+      <c r="D159" s="75"/>
+      <c r="E159" s="75"/>
     </row>
     <row r="160" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A160" s="75"/>
-      <c r="B160" s="73" t="s">
+      <c r="A160" s="90"/>
+      <c r="B160" s="97" t="s">
         <v>63</v>
       </c>
-      <c r="C160" s="75"/>
-      <c r="D160" s="98"/>
-      <c r="E160" s="98"/>
+      <c r="C160" s="90"/>
+      <c r="D160" s="81"/>
+      <c r="E160" s="81"/>
     </row>
     <row r="161" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A161" s="75"/>
+      <c r="A161" s="90"/>
       <c r="B161" s="41" t="s">
         <v>53</v>
       </c>
       <c r="C161" s="6">
         <v>4</v>
       </c>
-      <c r="D161" s="92"/>
-      <c r="E161" s="92"/>
+      <c r="D161" s="75"/>
+      <c r="E161" s="75"/>
     </row>
     <row r="162" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A162" s="75"/>
+      <c r="A162" s="90"/>
       <c r="B162" s="23" t="s">
         <v>64</v>
       </c>
       <c r="C162" s="6"/>
-      <c r="D162" s="92"/>
-      <c r="E162" s="92"/>
+      <c r="D162" s="75"/>
+      <c r="E162" s="75"/>
     </row>
     <row r="163" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A163" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="B163" s="74" t="s">
+      <c r="B163" s="103" t="s">
         <v>96</v>
       </c>
-      <c r="C163" s="74"/>
-      <c r="D163" s="99"/>
-      <c r="E163" s="99"/>
+      <c r="C163" s="103"/>
+      <c r="D163" s="82"/>
+      <c r="E163" s="82"/>
     </row>
     <row r="164" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A164" s="77" t="s">
+      <c r="A164" s="89" t="s">
         <v>65</v>
       </c>
       <c r="B164" s="40" t="s">
@@ -3437,60 +3437,60 @@
       <c r="C164" s="6">
         <v>8</v>
       </c>
-      <c r="D164" s="92"/>
-      <c r="E164" s="92"/>
+      <c r="D164" s="75"/>
+      <c r="E164" s="75"/>
     </row>
     <row r="165" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A165" s="75"/>
+      <c r="A165" s="90"/>
       <c r="B165" s="18" t="s">
         <v>118</v>
       </c>
       <c r="C165" s="6">
         <v>1</v>
       </c>
-      <c r="D165" s="92"/>
-      <c r="E165" s="92"/>
+      <c r="D165" s="75"/>
+      <c r="E165" s="75"/>
     </row>
     <row r="166" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A166" s="75"/>
-      <c r="B166" s="73" t="s">
+      <c r="A166" s="90"/>
+      <c r="B166" s="97" t="s">
         <v>63</v>
       </c>
-      <c r="C166" s="73"/>
-      <c r="D166" s="100"/>
-      <c r="E166" s="100"/>
+      <c r="C166" s="97"/>
+      <c r="D166" s="83"/>
+      <c r="E166" s="83"/>
     </row>
     <row r="167" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A167" s="75"/>
+      <c r="A167" s="90"/>
       <c r="B167" s="23" t="s">
         <v>66</v>
       </c>
       <c r="C167" s="6">
         <v>1</v>
       </c>
-      <c r="D167" s="92"/>
-      <c r="E167" s="92"/>
+      <c r="D167" s="75"/>
+      <c r="E167" s="75"/>
     </row>
     <row r="168" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A168" s="75"/>
+      <c r="A168" s="90"/>
       <c r="B168" s="23" t="s">
         <v>64</v>
       </c>
       <c r="C168" s="6"/>
-      <c r="D168" s="92"/>
-      <c r="E168" s="92"/>
+      <c r="D168" s="75"/>
+      <c r="E168" s="75"/>
     </row>
     <row r="169" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A169" s="75"/>
+      <c r="A169" s="90"/>
       <c r="B169" s="53" t="s">
         <v>46</v>
       </c>
       <c r="C169" s="64"/>
-      <c r="D169" s="97"/>
-      <c r="E169" s="97"/>
+      <c r="D169" s="80"/>
+      <c r="E169" s="80"/>
     </row>
     <row r="170" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A170" s="77" t="s">
+      <c r="A170" s="89" t="s">
         <v>67</v>
       </c>
       <c r="B170" s="23" t="s">
@@ -3499,33 +3499,33 @@
       <c r="C170" s="6">
         <v>0</v>
       </c>
-      <c r="D170" s="92"/>
-      <c r="E170" s="92"/>
+      <c r="D170" s="75"/>
+      <c r="E170" s="75"/>
     </row>
     <row r="171" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A171" s="75"/>
+      <c r="A171" s="90"/>
       <c r="B171" s="27" t="s">
         <v>103</v>
       </c>
       <c r="C171" s="6">
         <v>8</v>
       </c>
-      <c r="D171" s="92"/>
-      <c r="E171" s="92"/>
+      <c r="D171" s="75"/>
+      <c r="E171" s="75"/>
     </row>
     <row r="172" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A172" s="75"/>
+      <c r="A172" s="90"/>
       <c r="B172" s="40" t="s">
         <v>102</v>
       </c>
       <c r="C172" s="6">
         <v>6</v>
       </c>
-      <c r="D172" s="92"/>
-      <c r="E172" s="92"/>
+      <c r="D172" s="75"/>
+      <c r="E172" s="75"/>
     </row>
     <row r="173" spans="1:5" ht="31.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A173" s="77" t="s">
+      <c r="A173" s="89" t="s">
         <v>68</v>
       </c>
       <c r="B173" s="29" t="s">
@@ -3534,31 +3534,31 @@
       <c r="C173" s="6">
         <v>49</v>
       </c>
-      <c r="D173" s="92"/>
-      <c r="E173" s="92"/>
+      <c r="D173" s="75"/>
+      <c r="E173" s="75"/>
     </row>
     <row r="174" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A174" s="77"/>
+      <c r="A174" s="89"/>
       <c r="B174" s="41" t="s">
         <v>69</v>
       </c>
       <c r="C174" s="6">
         <v>4</v>
       </c>
-      <c r="D174" s="92"/>
-      <c r="E174" s="92"/>
+      <c r="D174" s="75"/>
+      <c r="E174" s="75"/>
     </row>
     <row r="175" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A175" s="75"/>
+      <c r="A175" s="90"/>
       <c r="B175" s="23" t="s">
         <v>64</v>
       </c>
       <c r="C175" s="3"/>
-      <c r="D175" s="98"/>
-      <c r="E175" s="98"/>
+      <c r="D175" s="81"/>
+      <c r="E175" s="81"/>
     </row>
     <row r="176" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A176" s="77" t="s">
+      <c r="A176" s="89" t="s">
         <v>70</v>
       </c>
       <c r="B176" s="40" t="s">
@@ -3567,64 +3567,64 @@
       <c r="C176" s="6">
         <v>4</v>
       </c>
-      <c r="D176" s="92"/>
-      <c r="E176" s="92"/>
+      <c r="D176" s="75"/>
+      <c r="E176" s="75"/>
     </row>
     <row r="177" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A177" s="75"/>
+      <c r="A177" s="90"/>
       <c r="B177" s="27" t="s">
         <v>103</v>
       </c>
       <c r="C177" s="6">
         <v>1</v>
       </c>
-      <c r="D177" s="92"/>
-      <c r="E177" s="92"/>
+      <c r="D177" s="75"/>
+      <c r="E177" s="75"/>
     </row>
     <row r="178" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A178" s="75"/>
+      <c r="A178" s="90"/>
       <c r="B178" s="22" t="s">
         <v>101</v>
       </c>
       <c r="C178" s="6">
         <v>3</v>
       </c>
-      <c r="D178" s="92"/>
-      <c r="E178" s="92"/>
+      <c r="D178" s="75"/>
+      <c r="E178" s="75"/>
     </row>
     <row r="179" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A179" s="75"/>
+      <c r="A179" s="90"/>
       <c r="B179" s="41" t="s">
         <v>50</v>
       </c>
       <c r="C179" s="6">
         <v>1</v>
       </c>
-      <c r="D179" s="92"/>
-      <c r="E179" s="92"/>
+      <c r="D179" s="75"/>
+      <c r="E179" s="75"/>
     </row>
     <row r="180" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A180" s="75"/>
+      <c r="A180" s="90"/>
       <c r="B180" s="23" t="s">
         <v>38</v>
       </c>
       <c r="C180" s="6">
         <v>1</v>
       </c>
-      <c r="D180" s="92"/>
-      <c r="E180" s="92"/>
+      <c r="D180" s="75"/>
+      <c r="E180" s="75"/>
     </row>
     <row r="181" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A181" s="75"/>
+      <c r="A181" s="90"/>
       <c r="B181" s="23" t="s">
         <v>43</v>
       </c>
       <c r="C181" s="6"/>
-      <c r="D181" s="92"/>
-      <c r="E181" s="92"/>
+      <c r="D181" s="75"/>
+      <c r="E181" s="75"/>
     </row>
     <row r="182" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A182" s="77" t="s">
+      <c r="A182" s="89" t="s">
         <v>71</v>
       </c>
       <c r="B182" s="24" t="s">
@@ -3633,95 +3633,95 @@
       <c r="C182" s="6">
         <v>74</v>
       </c>
-      <c r="D182" s="92"/>
-      <c r="E182" s="92"/>
+      <c r="D182" s="75"/>
+      <c r="E182" s="75"/>
     </row>
     <row r="183" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A183" s="75"/>
+      <c r="A183" s="90"/>
       <c r="B183" s="24" t="s">
         <v>129</v>
       </c>
       <c r="C183" s="6">
         <v>93</v>
       </c>
-      <c r="D183" s="92"/>
-      <c r="E183" s="92"/>
+      <c r="D183" s="75"/>
+      <c r="E183" s="75"/>
     </row>
     <row r="184" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A184" s="75"/>
+      <c r="A184" s="90"/>
       <c r="B184" s="27" t="s">
         <v>103</v>
       </c>
       <c r="C184" s="6">
         <v>38</v>
       </c>
-      <c r="D184" s="92"/>
-      <c r="E184" s="92"/>
+      <c r="D184" s="75"/>
+      <c r="E184" s="75"/>
     </row>
     <row r="185" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A185" s="75"/>
+      <c r="A185" s="90"/>
       <c r="B185" s="22" t="s">
         <v>101</v>
       </c>
       <c r="C185" s="6">
         <v>22</v>
       </c>
-      <c r="D185" s="92"/>
-      <c r="E185" s="92"/>
+      <c r="D185" s="75"/>
+      <c r="E185" s="75"/>
     </row>
     <row r="186" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A186" s="75"/>
+      <c r="A186" s="90"/>
       <c r="B186" s="13" t="s">
         <v>106</v>
       </c>
       <c r="C186" s="6">
         <v>6</v>
       </c>
-      <c r="D186" s="92"/>
-      <c r="E186" s="92"/>
+      <c r="D186" s="75"/>
+      <c r="E186" s="75"/>
     </row>
     <row r="187" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A187" s="75"/>
+      <c r="A187" s="90"/>
       <c r="B187" s="40" t="s">
         <v>102</v>
       </c>
       <c r="C187" s="6">
         <v>7</v>
       </c>
-      <c r="D187" s="92"/>
-      <c r="E187" s="92"/>
+      <c r="D187" s="75"/>
+      <c r="E187" s="75"/>
     </row>
     <row r="188" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A188" s="75"/>
+      <c r="A188" s="90"/>
       <c r="B188" s="23" t="s">
         <v>139</v>
       </c>
       <c r="C188" s="6">
         <v>1</v>
       </c>
-      <c r="D188" s="92"/>
-      <c r="E188" s="92"/>
+      <c r="D188" s="75"/>
+      <c r="E188" s="75"/>
     </row>
     <row r="189" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A189" s="75"/>
+      <c r="A189" s="90"/>
       <c r="B189" s="23" t="s">
         <v>43</v>
       </c>
       <c r="C189" s="6"/>
-      <c r="D189" s="92"/>
-      <c r="E189" s="92"/>
+      <c r="D189" s="75"/>
+      <c r="E189" s="75"/>
     </row>
     <row r="190" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A190" s="75"/>
+      <c r="A190" s="90"/>
       <c r="B190" s="53" t="s">
         <v>55</v>
       </c>
       <c r="C190" s="6"/>
-      <c r="D190" s="92"/>
-      <c r="E190" s="92"/>
+      <c r="D190" s="75"/>
+      <c r="E190" s="75"/>
     </row>
     <row r="191" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A191" s="77" t="s">
+      <c r="A191" s="89" t="s">
         <v>72</v>
       </c>
       <c r="B191" s="32" t="s">
@@ -3730,152 +3730,152 @@
       <c r="C191" s="6">
         <v>11</v>
       </c>
-      <c r="D191" s="92"/>
-      <c r="E191" s="92"/>
+      <c r="D191" s="75"/>
+      <c r="E191" s="75"/>
     </row>
     <row r="192" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A192" s="75"/>
+      <c r="A192" s="90"/>
       <c r="B192" s="27" t="s">
         <v>103</v>
       </c>
       <c r="C192" s="6">
         <v>24</v>
       </c>
-      <c r="D192" s="92"/>
-      <c r="E192" s="92"/>
+      <c r="D192" s="75"/>
+      <c r="E192" s="75"/>
     </row>
     <row r="193" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A193" s="75"/>
+      <c r="A193" s="90"/>
       <c r="B193" s="33" t="s">
         <v>73</v>
       </c>
       <c r="C193" s="6">
         <v>13</v>
       </c>
-      <c r="D193" s="92"/>
-      <c r="E193" s="92"/>
+      <c r="D193" s="75"/>
+      <c r="E193" s="75"/>
     </row>
     <row r="194" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A194" s="75"/>
+      <c r="A194" s="90"/>
       <c r="B194" s="40" t="s">
         <v>102</v>
       </c>
       <c r="C194" s="6">
         <v>4</v>
       </c>
-      <c r="D194" s="92"/>
-      <c r="E194" s="92"/>
+      <c r="D194" s="75"/>
+      <c r="E194" s="75"/>
     </row>
     <row r="195" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A195" s="75"/>
+      <c r="A195" s="90"/>
       <c r="B195" s="41" t="s">
         <v>74</v>
       </c>
       <c r="C195" s="6">
         <v>1</v>
       </c>
-      <c r="D195" s="92"/>
-      <c r="E195" s="92"/>
+      <c r="D195" s="75"/>
+      <c r="E195" s="75"/>
     </row>
     <row r="196" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A196" s="75"/>
+      <c r="A196" s="90"/>
       <c r="B196" s="34" t="s">
         <v>159</v>
       </c>
       <c r="C196" s="6">
         <v>7</v>
       </c>
-      <c r="D196" s="92"/>
-      <c r="E196" s="92"/>
+      <c r="D196" s="75"/>
+      <c r="E196" s="75"/>
     </row>
     <row r="197" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A197" s="75"/>
+      <c r="A197" s="90"/>
       <c r="B197" s="41" t="s">
         <v>75</v>
       </c>
       <c r="C197" s="6">
         <v>4</v>
       </c>
-      <c r="D197" s="92"/>
-      <c r="E197" s="92"/>
+      <c r="D197" s="75"/>
+      <c r="E197" s="75"/>
     </row>
     <row r="198" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A198" s="75"/>
+      <c r="A198" s="90"/>
       <c r="B198" s="41" t="s">
         <v>76</v>
       </c>
       <c r="C198" s="6">
         <v>20</v>
       </c>
-      <c r="D198" s="92"/>
-      <c r="E198" s="92"/>
+      <c r="D198" s="75"/>
+      <c r="E198" s="75"/>
     </row>
     <row r="199" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A199" s="75"/>
+      <c r="A199" s="90"/>
       <c r="B199" s="41" t="s">
         <v>77</v>
       </c>
       <c r="C199" s="6">
         <v>1</v>
       </c>
-      <c r="D199" s="92"/>
-      <c r="E199" s="92"/>
+      <c r="D199" s="75"/>
+      <c r="E199" s="75"/>
     </row>
     <row r="200" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A200" s="75"/>
+      <c r="A200" s="90"/>
       <c r="B200" s="9" t="s">
         <v>105</v>
       </c>
       <c r="C200" s="6">
         <v>1</v>
       </c>
-      <c r="D200" s="92"/>
-      <c r="E200" s="92"/>
+      <c r="D200" s="75"/>
+      <c r="E200" s="75"/>
     </row>
     <row r="201" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A201" s="75"/>
+      <c r="A201" s="90"/>
       <c r="B201" s="24" t="s">
         <v>104</v>
       </c>
       <c r="C201" s="6">
         <v>8</v>
       </c>
-      <c r="D201" s="92"/>
-      <c r="E201" s="92"/>
+      <c r="D201" s="75"/>
+      <c r="E201" s="75"/>
     </row>
     <row r="202" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A202" s="75"/>
+      <c r="A202" s="90"/>
       <c r="B202" s="17" t="s">
         <v>115</v>
       </c>
       <c r="C202" s="6">
         <v>3</v>
       </c>
-      <c r="D202" s="92"/>
-      <c r="E202" s="92"/>
+      <c r="D202" s="75"/>
+      <c r="E202" s="75"/>
     </row>
     <row r="203" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A203" s="75"/>
+      <c r="A203" s="90"/>
       <c r="B203" s="41" t="s">
         <v>53</v>
       </c>
       <c r="C203" s="6">
         <v>1</v>
       </c>
-      <c r="D203" s="92"/>
-      <c r="E203" s="92"/>
+      <c r="D203" s="75"/>
+      <c r="E203" s="75"/>
     </row>
     <row r="204" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A204" s="75"/>
+      <c r="A204" s="90"/>
       <c r="B204" s="53" t="s">
         <v>55</v>
       </c>
       <c r="C204" s="6"/>
-      <c r="D204" s="92"/>
-      <c r="E204" s="92"/>
+      <c r="D204" s="75"/>
+      <c r="E204" s="75"/>
     </row>
     <row r="205" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A205" s="77" t="s">
+      <c r="A205" s="89" t="s">
         <v>78</v>
       </c>
       <c r="B205" s="40" t="s">
@@ -3884,99 +3884,99 @@
       <c r="C205" s="6">
         <v>12</v>
       </c>
-      <c r="D205" s="92"/>
-      <c r="E205" s="92"/>
+      <c r="D205" s="75"/>
+      <c r="E205" s="75"/>
     </row>
     <row r="206" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A206" s="75"/>
+      <c r="A206" s="90"/>
       <c r="B206" s="27" t="s">
         <v>103</v>
       </c>
       <c r="C206" s="6">
         <v>6</v>
       </c>
-      <c r="D206" s="92"/>
-      <c r="E206" s="92"/>
+      <c r="D206" s="75"/>
+      <c r="E206" s="75"/>
     </row>
     <row r="207" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A207" s="75"/>
+      <c r="A207" s="90"/>
       <c r="B207" s="24" t="s">
         <v>104</v>
       </c>
       <c r="C207" s="6">
         <v>5</v>
       </c>
-      <c r="D207" s="92"/>
-      <c r="E207" s="92"/>
+      <c r="D207" s="75"/>
+      <c r="E207" s="75"/>
     </row>
     <row r="208" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A208" s="75"/>
+      <c r="A208" s="90"/>
       <c r="B208" s="22" t="s">
         <v>101</v>
       </c>
       <c r="C208" s="6">
         <v>13</v>
       </c>
-      <c r="D208" s="92"/>
-      <c r="E208" s="92"/>
+      <c r="D208" s="75"/>
+      <c r="E208" s="75"/>
     </row>
     <row r="209" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A209" s="75"/>
+      <c r="A209" s="90"/>
       <c r="B209" s="33" t="s">
         <v>139</v>
       </c>
       <c r="C209" s="6">
         <v>1</v>
       </c>
-      <c r="D209" s="92"/>
-      <c r="E209" s="92"/>
+      <c r="D209" s="75"/>
+      <c r="E209" s="75"/>
     </row>
     <row r="210" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A210" s="75"/>
+      <c r="A210" s="90"/>
       <c r="B210" s="9" t="s">
         <v>105</v>
       </c>
       <c r="C210" s="6">
         <v>1</v>
       </c>
-      <c r="D210" s="92"/>
-      <c r="E210" s="92"/>
+      <c r="D210" s="75"/>
+      <c r="E210" s="75"/>
     </row>
     <row r="211" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A211" s="75"/>
+      <c r="A211" s="90"/>
       <c r="B211" s="11" t="s">
         <v>125</v>
       </c>
       <c r="C211" s="6">
         <v>1</v>
       </c>
-      <c r="D211" s="92"/>
-      <c r="E211" s="92"/>
+      <c r="D211" s="75"/>
+      <c r="E211" s="75"/>
     </row>
     <row r="212" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A212" s="75"/>
+      <c r="A212" s="90"/>
       <c r="B212" s="20" t="s">
         <v>118</v>
       </c>
       <c r="C212" s="6">
         <v>6</v>
       </c>
-      <c r="D212" s="92"/>
-      <c r="E212" s="92"/>
+      <c r="D212" s="75"/>
+      <c r="E212" s="75"/>
     </row>
     <row r="213" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A213" s="75"/>
+      <c r="A213" s="90"/>
       <c r="B213" s="41" t="s">
         <v>79</v>
       </c>
       <c r="C213" s="6">
         <v>1</v>
       </c>
-      <c r="D213" s="92"/>
-      <c r="E213" s="92"/>
+      <c r="D213" s="75"/>
+      <c r="E213" s="75"/>
     </row>
     <row r="214" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A214" s="77" t="s">
+      <c r="A214" s="89" t="s">
         <v>80</v>
       </c>
       <c r="B214" s="27" t="s">
@@ -3985,225 +3985,225 @@
       <c r="C214" s="6">
         <v>24</v>
       </c>
-      <c r="D214" s="92"/>
-      <c r="E214" s="92"/>
+      <c r="D214" s="75"/>
+      <c r="E214" s="75"/>
     </row>
     <row r="215" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A215" s="75"/>
+      <c r="A215" s="90"/>
       <c r="B215" s="43" t="s">
         <v>114</v>
       </c>
       <c r="C215" s="6">
         <v>4</v>
       </c>
-      <c r="D215" s="92"/>
-      <c r="E215" s="92"/>
+      <c r="D215" s="75"/>
+      <c r="E215" s="75"/>
     </row>
     <row r="216" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A216" s="75"/>
+      <c r="A216" s="90"/>
       <c r="B216" s="33" t="s">
         <v>38</v>
       </c>
       <c r="C216" s="6">
         <v>2</v>
       </c>
-      <c r="D216" s="92"/>
-      <c r="E216" s="92"/>
+      <c r="D216" s="75"/>
+      <c r="E216" s="75"/>
     </row>
     <row r="217" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A217" s="75"/>
+      <c r="A217" s="90"/>
       <c r="B217" s="40" t="s">
         <v>102</v>
       </c>
       <c r="C217" s="6">
         <v>6</v>
       </c>
-      <c r="D217" s="92"/>
-      <c r="E217" s="92"/>
+      <c r="D217" s="75"/>
+      <c r="E217" s="75"/>
     </row>
     <row r="218" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A218" s="75"/>
+      <c r="A218" s="90"/>
       <c r="B218" s="24" t="s">
         <v>104</v>
       </c>
       <c r="C218" s="6">
         <v>3</v>
       </c>
-      <c r="D218" s="92"/>
-      <c r="E218" s="92"/>
+      <c r="D218" s="75"/>
+      <c r="E218" s="75"/>
     </row>
     <row r="219" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A219" s="75"/>
+      <c r="A219" s="90"/>
       <c r="B219" s="41" t="s">
         <v>26</v>
       </c>
       <c r="C219" s="6">
         <v>1</v>
       </c>
-      <c r="D219" s="92"/>
-      <c r="E219" s="92"/>
+      <c r="D219" s="75"/>
+      <c r="E219" s="75"/>
     </row>
     <row r="220" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A220" s="75"/>
+      <c r="A220" s="90"/>
       <c r="B220" s="22" t="s">
         <v>101</v>
       </c>
       <c r="C220" s="6">
         <v>2</v>
       </c>
-      <c r="D220" s="92"/>
-      <c r="E220" s="92"/>
+      <c r="D220" s="75"/>
+      <c r="E220" s="75"/>
     </row>
     <row r="221" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A221" s="75"/>
+      <c r="A221" s="90"/>
       <c r="B221" s="30" t="s">
         <v>107</v>
       </c>
       <c r="C221" s="6">
         <v>25</v>
       </c>
-      <c r="D221" s="92"/>
-      <c r="E221" s="92"/>
+      <c r="D221" s="75"/>
+      <c r="E221" s="75"/>
     </row>
     <row r="222" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A222" s="75"/>
+      <c r="A222" s="90"/>
       <c r="B222" s="25" t="s">
         <v>137</v>
       </c>
       <c r="C222" s="6">
         <v>2</v>
       </c>
-      <c r="D222" s="92"/>
-      <c r="E222" s="92"/>
+      <c r="D222" s="75"/>
+      <c r="E222" s="75"/>
     </row>
     <row r="223" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A223" s="75"/>
+      <c r="A223" s="90"/>
       <c r="B223" s="12" t="s">
         <v>110</v>
       </c>
       <c r="C223" s="6">
         <v>2</v>
       </c>
-      <c r="D223" s="92"/>
-      <c r="E223" s="92"/>
+      <c r="D223" s="75"/>
+      <c r="E223" s="75"/>
     </row>
     <row r="224" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A224" s="75"/>
-      <c r="B224" s="73" t="s">
+      <c r="A224" s="90"/>
+      <c r="B224" s="97" t="s">
         <v>59</v>
       </c>
-      <c r="C224" s="73"/>
-      <c r="D224" s="100"/>
-      <c r="E224" s="100"/>
+      <c r="C224" s="97"/>
+      <c r="D224" s="83"/>
+      <c r="E224" s="83"/>
     </row>
     <row r="225" spans="1:6" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A225" s="75"/>
+      <c r="A225" s="90"/>
       <c r="B225" s="47" t="s">
         <v>142</v>
       </c>
       <c r="C225" s="7">
         <v>1</v>
       </c>
-      <c r="D225" s="91"/>
-      <c r="E225" s="91"/>
+      <c r="D225" s="74"/>
+      <c r="E225" s="74"/>
     </row>
     <row r="226" spans="1:6" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A226" s="75"/>
+      <c r="A226" s="90"/>
       <c r="B226" s="41" t="s">
         <v>119</v>
       </c>
       <c r="C226" s="7">
         <v>2</v>
       </c>
-      <c r="D226" s="91"/>
-      <c r="E226" s="91"/>
+      <c r="D226" s="74"/>
+      <c r="E226" s="74"/>
     </row>
     <row r="227" spans="1:6" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A227" s="75"/>
+      <c r="A227" s="90"/>
       <c r="B227" s="9" t="s">
         <v>105</v>
       </c>
       <c r="C227" s="7">
         <v>2</v>
       </c>
-      <c r="D227" s="91"/>
-      <c r="E227" s="91"/>
+      <c r="D227" s="74"/>
+      <c r="E227" s="74"/>
     </row>
     <row r="228" spans="1:6" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A228" s="75"/>
+      <c r="A228" s="90"/>
       <c r="B228" s="53" t="s">
         <v>81</v>
       </c>
       <c r="C228" s="53"/>
-      <c r="D228" s="101"/>
-      <c r="E228" s="101"/>
+      <c r="D228" s="84"/>
+      <c r="E228" s="84"/>
     </row>
     <row r="229" spans="1:6" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A229" s="75"/>
+      <c r="A229" s="90"/>
       <c r="B229" s="53" t="s">
         <v>116</v>
       </c>
       <c r="C229" s="55">
         <v>1</v>
       </c>
-      <c r="D229" s="102"/>
-      <c r="E229" s="102"/>
+      <c r="D229" s="85"/>
+      <c r="E229" s="85"/>
     </row>
     <row r="230" spans="1:6" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A230" s="75"/>
+      <c r="A230" s="90"/>
       <c r="B230" s="53" t="s">
         <v>82</v>
       </c>
       <c r="C230" s="55">
         <v>1</v>
       </c>
-      <c r="D230" s="102"/>
-      <c r="E230" s="102"/>
+      <c r="D230" s="85"/>
+      <c r="E230" s="85"/>
     </row>
     <row r="231" spans="1:6" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A231" s="75"/>
+      <c r="A231" s="90"/>
       <c r="B231" s="53" t="s">
         <v>115</v>
       </c>
       <c r="C231" s="55">
         <v>2</v>
       </c>
-      <c r="D231" s="102"/>
-      <c r="E231" s="102"/>
+      <c r="D231" s="85"/>
+      <c r="E231" s="85"/>
     </row>
     <row r="232" spans="1:6" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A232" s="75"/>
+      <c r="A232" s="90"/>
       <c r="B232" s="53" t="s">
         <v>83</v>
       </c>
       <c r="C232" s="55">
         <v>2</v>
       </c>
-      <c r="D232" s="102"/>
-      <c r="E232" s="102"/>
+      <c r="D232" s="85"/>
+      <c r="E232" s="85"/>
     </row>
     <row r="233" spans="1:6" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A233" s="75"/>
+      <c r="A233" s="90"/>
       <c r="B233" s="23" t="s">
         <v>84</v>
       </c>
       <c r="C233" s="6">
         <v>4</v>
       </c>
-      <c r="D233" s="92"/>
-      <c r="E233" s="92"/>
+      <c r="D233" s="75"/>
+      <c r="E233" s="75"/>
     </row>
     <row r="234" spans="1:6" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A234" s="75"/>
+      <c r="A234" s="90"/>
       <c r="B234" s="23" t="s">
         <v>85</v>
       </c>
       <c r="C234" s="6"/>
-      <c r="D234" s="92"/>
-      <c r="E234" s="92"/>
+      <c r="D234" s="75"/>
+      <c r="E234" s="75"/>
     </row>
     <row r="235" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A235" s="80" t="s">
+      <c r="A235" s="98" t="s">
         <v>160</v>
       </c>
       <c r="B235" s="49" t="s">
@@ -4212,28 +4212,28 @@
       <c r="C235" s="6">
         <v>3</v>
       </c>
-      <c r="D235" s="92"/>
-      <c r="E235" s="92"/>
+      <c r="D235" s="75"/>
+      <c r="E235" s="75"/>
     </row>
     <row r="236" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A236" s="80"/>
+      <c r="A236" s="98"/>
       <c r="B236" s="11" t="s">
         <v>125</v>
       </c>
       <c r="C236" s="6">
         <v>1</v>
       </c>
-      <c r="D236" s="92"/>
-      <c r="E236" s="92"/>
+      <c r="D236" s="75"/>
+      <c r="E236" s="75"/>
     </row>
     <row r="237" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A237" s="80"/>
+      <c r="A237" s="98"/>
       <c r="B237" s="56" t="s">
         <v>46</v>
       </c>
       <c r="C237" s="6"/>
-      <c r="D237" s="92"/>
-      <c r="E237" s="92"/>
+      <c r="D237" s="75"/>
+      <c r="E237" s="75"/>
     </row>
     <row r="238" spans="1:6" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A238" s="1" t="s">
@@ -4245,8 +4245,8 @@
       <c r="C238" s="6">
         <v>12</v>
       </c>
-      <c r="D238" s="92"/>
-      <c r="E238" s="92"/>
+      <c r="D238" s="75"/>
+      <c r="E238" s="75"/>
     </row>
     <row r="239" spans="1:6" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A239" s="1" t="s">
@@ -4258,12 +4258,12 @@
       <c r="C239" s="6">
         <v>1</v>
       </c>
-      <c r="D239" s="92"/>
-      <c r="E239" s="92"/>
+      <c r="D239" s="75"/>
+      <c r="E239" s="75"/>
     </row>
     <row r="240" spans="1:6" s="70" customFormat="1" ht="78.75" x14ac:dyDescent="0.2">
       <c r="A240" s="66" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B240" s="41" t="s">
         <v>88</v>
@@ -4271,10 +4271,10 @@
       <c r="C240" s="65">
         <v>5</v>
       </c>
-      <c r="D240" s="92"/>
-      <c r="E240" s="92"/>
-      <c r="F240" s="92" t="s">
-        <v>174</v>
+      <c r="D240" s="75"/>
+      <c r="E240" s="75"/>
+      <c r="F240" s="75" t="s">
+        <v>173</v>
       </c>
     </row>
     <row r="241" spans="1:6" ht="15.75" x14ac:dyDescent="0.2">
@@ -4287,8 +4287,8 @@
       <c r="C241" s="6">
         <v>3</v>
       </c>
-      <c r="D241" s="92"/>
-      <c r="E241" s="92"/>
+      <c r="D241" s="75"/>
+      <c r="E241" s="75"/>
       <c r="F241" s="70"/>
     </row>
     <row r="242" spans="1:6" ht="27" x14ac:dyDescent="0.2">
@@ -4301,8 +4301,8 @@
       <c r="C242" s="7" t="s">
         <v>165</v>
       </c>
-      <c r="D242" s="91"/>
-      <c r="E242" s="91"/>
+      <c r="D242" s="74"/>
+      <c r="E242" s="74"/>
     </row>
     <row r="243" spans="1:6" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A243" s="1" t="s">
@@ -4310,58 +4310,58 @@
       </c>
       <c r="B243" s="23"/>
       <c r="C243" s="7"/>
-      <c r="D243" s="91"/>
-      <c r="E243" s="91"/>
+      <c r="D243" s="74"/>
+      <c r="E243" s="74"/>
     </row>
     <row r="244" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A244" s="3"/>
-      <c r="B244" s="82" t="s">
+      <c r="B244" s="100" t="s">
         <v>120</v>
       </c>
-      <c r="C244" s="85">
+      <c r="C244" s="91">
         <f>SUM(C229:C242,C225:C227,C167:C223,C164:C165,C161,C148:C159,C10:C146)</f>
-        <v>2019</v>
-      </c>
-      <c r="D244" s="103"/>
-      <c r="E244" s="103"/>
+        <v>2022</v>
+      </c>
+      <c r="D244" s="86"/>
+      <c r="E244" s="86"/>
     </row>
     <row r="245" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A245" s="3"/>
-      <c r="B245" s="82"/>
-      <c r="C245" s="86"/>
-      <c r="D245" s="103"/>
-      <c r="E245" s="103"/>
+      <c r="B245" s="100"/>
+      <c r="C245" s="92"/>
+      <c r="D245" s="86"/>
+      <c r="E245" s="86"/>
     </row>
     <row r="246" spans="1:6" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A246" s="81"/>
-      <c r="B246" s="81"/>
-      <c r="C246" s="81"/>
-      <c r="D246" s="104"/>
-      <c r="E246" s="104"/>
+      <c r="A246" s="99"/>
+      <c r="B246" s="99"/>
+      <c r="C246" s="99"/>
+      <c r="D246" s="87"/>
+      <c r="E246" s="87"/>
     </row>
     <row r="247" spans="1:6" ht="31.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A247" s="78"/>
-      <c r="B247" s="78"/>
-      <c r="C247" s="78"/>
+      <c r="A247" s="95"/>
+      <c r="B247" s="95"/>
+      <c r="C247" s="95"/>
       <c r="D247" s="67"/>
       <c r="E247" s="67"/>
     </row>
     <row r="248" spans="1:6" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A248" s="78"/>
-      <c r="B248" s="78"/>
-      <c r="C248" s="78"/>
+      <c r="A248" s="95"/>
+      <c r="B248" s="95"/>
+      <c r="C248" s="95"/>
       <c r="D248" s="67"/>
       <c r="E248" s="67"/>
     </row>
     <row r="249" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A249" s="78"/>
+      <c r="A249" s="95"/>
       <c r="B249" s="57"/>
       <c r="C249" s="50"/>
       <c r="D249" s="68"/>
       <c r="E249" s="68"/>
     </row>
     <row r="250" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A250" s="79"/>
+      <c r="A250" s="96"/>
       <c r="B250" s="57"/>
       <c r="C250" s="50"/>
       <c r="D250" s="68"/>
@@ -4423,6 +4423,39 @@
     </row>
   </sheetData>
   <mergeCells count="49">
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="A3:C3"/>
+    <mergeCell ref="B166:C166"/>
+    <mergeCell ref="B163:C163"/>
+    <mergeCell ref="B160:C160"/>
+    <mergeCell ref="C65:C66"/>
+    <mergeCell ref="B147:C147"/>
+    <mergeCell ref="A26:A27"/>
+    <mergeCell ref="A139:A151"/>
+    <mergeCell ref="A154:A162"/>
+    <mergeCell ref="A105:A125"/>
+    <mergeCell ref="A164:A169"/>
+    <mergeCell ref="A191:A204"/>
+    <mergeCell ref="A248:C248"/>
+    <mergeCell ref="A249:A250"/>
+    <mergeCell ref="A214:A234"/>
+    <mergeCell ref="B224:C224"/>
+    <mergeCell ref="A235:A237"/>
+    <mergeCell ref="A246:C246"/>
+    <mergeCell ref="A247:C247"/>
+    <mergeCell ref="B244:B245"/>
+    <mergeCell ref="A205:A213"/>
+    <mergeCell ref="A170:A172"/>
+    <mergeCell ref="A173:A175"/>
+    <mergeCell ref="A182:A190"/>
+    <mergeCell ref="A176:A181"/>
+    <mergeCell ref="A52:A53"/>
+    <mergeCell ref="A65:A66"/>
+    <mergeCell ref="A78:A80"/>
+    <mergeCell ref="A81:A83"/>
+    <mergeCell ref="A126:A138"/>
+    <mergeCell ref="A97:A99"/>
+    <mergeCell ref="A100:A104"/>
     <mergeCell ref="A4:F8"/>
     <mergeCell ref="A29:A31"/>
     <mergeCell ref="A32:A33"/>
@@ -4439,39 +4472,6 @@
     <mergeCell ref="A55:A56"/>
     <mergeCell ref="A59:A62"/>
     <mergeCell ref="A49:A51"/>
-    <mergeCell ref="A52:A53"/>
-    <mergeCell ref="A65:A66"/>
-    <mergeCell ref="A78:A80"/>
-    <mergeCell ref="A81:A83"/>
-    <mergeCell ref="A126:A138"/>
-    <mergeCell ref="A97:A99"/>
-    <mergeCell ref="A100:A104"/>
-    <mergeCell ref="A205:A213"/>
-    <mergeCell ref="A170:A172"/>
-    <mergeCell ref="A173:A175"/>
-    <mergeCell ref="A182:A190"/>
-    <mergeCell ref="A176:A181"/>
-    <mergeCell ref="A164:A169"/>
-    <mergeCell ref="A191:A204"/>
-    <mergeCell ref="A248:C248"/>
-    <mergeCell ref="A249:A250"/>
-    <mergeCell ref="A214:A234"/>
-    <mergeCell ref="B224:C224"/>
-    <mergeCell ref="A235:A237"/>
-    <mergeCell ref="A246:C246"/>
-    <mergeCell ref="A247:C247"/>
-    <mergeCell ref="B244:B245"/>
-    <mergeCell ref="A2:C2"/>
-    <mergeCell ref="A3:C3"/>
-    <mergeCell ref="B166:C166"/>
-    <mergeCell ref="B163:C163"/>
-    <mergeCell ref="B160:C160"/>
-    <mergeCell ref="C65:C66"/>
-    <mergeCell ref="B147:C147"/>
-    <mergeCell ref="A26:A27"/>
-    <mergeCell ref="A139:A151"/>
-    <mergeCell ref="A154:A162"/>
-    <mergeCell ref="A105:A125"/>
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <printOptions horizontalCentered="1"/>

</xml_diff>